<commit_message>
Basic anomaly detection set up
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -393,15 +393,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>time_of_day</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>interval</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>num_sessions</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>milk_vol</t>
         </is>
@@ -415,22 +420,25 @@
         <v>43831.25</v>
       </c>
       <c r="C2" t="n">
-        <v>23.9750316242332</v>
+        <v>36.01431347021487</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
-        <v>4.430926160653468</v>
+        <v>4.67162667964305</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>20.43591870213761</v>
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>36.72921621003871</v>
       </c>
     </row>
     <row r="3">
@@ -441,22 +449,25 @@
         <v>43831.33333333334</v>
       </c>
       <c r="C3" t="n">
-        <v>35.32568832419058</v>
+        <v>37.09867410269293</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>5.873318740943508</v>
+        <v>2.669426998147992</v>
       </c>
       <c r="F3" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H3" t="n">
-        <v>36.76802133231192</v>
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>38.40672663825167</v>
       </c>
     </row>
     <row r="4">
@@ -467,22 +478,25 @@
         <v>43831.41666666666</v>
       </c>
       <c r="C4" t="n">
-        <v>39.28439139007247</v>
+        <v>21.21368086043092</v>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>4.757934646397577</v>
+        <v>9.540087842674083</v>
       </c>
       <c r="F4" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H4" t="n">
-        <v>37.98921832102207</v>
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>26.9284090717723</v>
       </c>
     </row>
     <row r="5">
@@ -493,22 +507,25 @@
         <v>43831.5</v>
       </c>
       <c r="C5" t="n">
-        <v>23.5112760709045</v>
+        <v>21.8668645652952</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>9.665981792451289</v>
+        <v>5.551821393422407</v>
       </c>
       <c r="F5" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H5" t="n">
-        <v>22.80808647966136</v>
+        <v>3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>22.26291833573902</v>
       </c>
     </row>
     <row r="6">
@@ -519,22 +536,25 @@
         <v>43831.58333333334</v>
       </c>
       <c r="C6" t="n">
-        <v>15.7228115286161</v>
+        <v>29.80060143478785</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>4.819346060966027</v>
+        <v>4.681249872197312</v>
       </c>
       <c r="F6" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
+        <v>120</v>
+      </c>
+      <c r="H6" t="n">
         <v>4</v>
       </c>
-      <c r="H6" t="n">
-        <v>20.21618232167006</v>
+      <c r="I6" t="n">
+        <v>24.73188914833978</v>
       </c>
     </row>
     <row r="7">
@@ -545,22 +565,25 @@
         <v>43831.66666666666</v>
       </c>
       <c r="C7" t="n">
-        <v>15.14029324746456</v>
+        <v>18.57714382720681</v>
       </c>
       <c r="D7" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>5.316869673659488</v>
+        <v>6.581310272734696</v>
       </c>
       <c r="F7" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
+        <v>120</v>
+      </c>
+      <c r="H7" t="n">
         <v>5</v>
       </c>
-      <c r="H7" t="n">
-        <v>12.38763494495256</v>
+      <c r="I7" t="n">
+        <v>16.82511192327269</v>
       </c>
     </row>
     <row r="8">
@@ -571,22 +594,25 @@
         <v>43831.75</v>
       </c>
       <c r="C8" t="n">
-        <v>30.1910292867953</v>
+        <v>31.16778923267143</v>
       </c>
       <c r="D8" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>5.333469650114201</v>
+        <v>3.238849856804833</v>
       </c>
       <c r="F8" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
+        <v>120</v>
+      </c>
+      <c r="H8" t="n">
         <v>6</v>
       </c>
-      <c r="H8" t="n">
-        <v>31.13193613920104</v>
+      <c r="I8" t="n">
+        <v>36.24767890788262</v>
       </c>
     </row>
     <row r="9">
@@ -597,22 +623,25 @@
         <v>43831.83333333334</v>
       </c>
       <c r="C9" t="n">
-        <v>36.2212468061453</v>
+        <v>30.55742128876495</v>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>8.557881441690926</v>
+        <v>7.271225825803306</v>
       </c>
       <c r="F9" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G9" t="n">
+        <v>120</v>
+      </c>
+      <c r="H9" t="n">
         <v>7</v>
       </c>
-      <c r="H9" t="n">
-        <v>39.78260030490021</v>
+      <c r="I9" t="n">
+        <v>30.58564636608049</v>
       </c>
     </row>
     <row r="10">
@@ -623,22 +652,25 @@
         <v>43832.25</v>
       </c>
       <c r="C10" t="n">
-        <v>21.1911477369801</v>
+        <v>26.37731220690105</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>9.042811769521768</v>
+        <v>2.012433622155277</v>
       </c>
       <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
         <v>600</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0</v>
       </c>
-      <c r="H10" t="n">
-        <v>20.84043052038531</v>
+      <c r="I10" t="n">
+        <v>28.65083262824011</v>
       </c>
     </row>
     <row r="11">
@@ -649,22 +681,25 @@
         <v>43832.33333333334</v>
       </c>
       <c r="C11" t="n">
-        <v>37.17044204117286</v>
+        <v>27.18329900415646</v>
       </c>
       <c r="D11" t="n">
         <v>11</v>
       </c>
       <c r="E11" t="n">
-        <v>2.494408181283108</v>
+        <v>9.750657050699456</v>
       </c>
       <c r="F11" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H11" t="n">
-        <v>29.53029853720938</v>
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>30.49897075391046</v>
       </c>
     </row>
     <row r="12">
@@ -675,22 +710,25 @@
         <v>43832.41666666666</v>
       </c>
       <c r="C12" t="n">
-        <v>22.22422484290979</v>
+        <v>16.59014954176223</v>
       </c>
       <c r="D12" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5.351535332698345</v>
+        <v>6.075182159520814</v>
       </c>
       <c r="F12" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H12" t="n">
-        <v>16.15971721615147</v>
+        <v>2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>17.85197780561959</v>
       </c>
     </row>
     <row r="13">
@@ -701,22 +739,25 @@
         <v>43832.5</v>
       </c>
       <c r="C13" t="n">
-        <v>38.96731872244796</v>
+        <v>17.18802836669729</v>
       </c>
       <c r="D13" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E13" t="n">
-        <v>3.108518932865207</v>
+        <v>3.475634059427983</v>
       </c>
       <c r="F13" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H13" t="n">
-        <v>36.5574276430739</v>
+        <v>3</v>
+      </c>
+      <c r="I13" t="n">
+        <v>18.1811749412619</v>
       </c>
     </row>
     <row r="14">
@@ -727,22 +768,25 @@
         <v>43832.58333333334</v>
       </c>
       <c r="C14" t="n">
-        <v>35.26378919456694</v>
+        <v>35.09312148435112</v>
       </c>
       <c r="D14" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E14" t="n">
-        <v>8.947487771291916</v>
+        <v>5.636320957802172</v>
       </c>
       <c r="F14" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
+        <v>120</v>
+      </c>
+      <c r="H14" t="n">
         <v>4</v>
       </c>
-      <c r="H14" t="n">
-        <v>35.71484385242874</v>
+      <c r="I14" t="n">
+        <v>32.53955757912584</v>
       </c>
     </row>
     <row r="15">
@@ -753,22 +797,25 @@
         <v>43832.66666666666</v>
       </c>
       <c r="C15" t="n">
-        <v>39.6054083495237</v>
+        <v>32.09246747936827</v>
       </c>
       <c r="D15" t="n">
         <v>9</v>
       </c>
       <c r="E15" t="n">
-        <v>8.382592187753925</v>
+        <v>6.642078373284341</v>
       </c>
       <c r="F15" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
+        <v>120</v>
+      </c>
+      <c r="H15" t="n">
         <v>5</v>
       </c>
-      <c r="H15" t="n">
-        <v>42.04795994507167</v>
+      <c r="I15" t="n">
+        <v>31.99225212192251</v>
       </c>
     </row>
     <row r="16">
@@ -779,22 +826,25 @@
         <v>43832.75</v>
       </c>
       <c r="C16" t="n">
-        <v>30.19129102457939</v>
+        <v>31.03659523036038</v>
       </c>
       <c r="D16" t="n">
         <v>3</v>
       </c>
       <c r="E16" t="n">
-        <v>5.865135243378389</v>
+        <v>5.356561634697422</v>
       </c>
       <c r="F16" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G16" t="n">
+        <v>120</v>
+      </c>
+      <c r="H16" t="n">
         <v>6</v>
       </c>
-      <c r="H16" t="n">
-        <v>28.26115456372337</v>
+      <c r="I16" t="n">
+        <v>31.52248477945314</v>
       </c>
     </row>
     <row r="17">
@@ -805,22 +855,25 @@
         <v>43832.83333333334</v>
       </c>
       <c r="C17" t="n">
-        <v>21.7516207543289</v>
+        <v>33.27638104073343</v>
       </c>
       <c r="D17" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>6.118426464914198</v>
+        <v>8.450378224785688</v>
       </c>
       <c r="F17" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G17" t="n">
+        <v>120</v>
+      </c>
+      <c r="H17" t="n">
         <v>7</v>
       </c>
-      <c r="H17" t="n">
-        <v>14.38138414005613</v>
+      <c r="I17" t="n">
+        <v>34.76057189654938</v>
       </c>
     </row>
     <row r="18">
@@ -831,22 +884,25 @@
         <v>43833.25</v>
       </c>
       <c r="C18" t="n">
-        <v>28.21811011785427</v>
+        <v>16.20053603057802</v>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" t="n">
-        <v>3.567467940931608</v>
+        <v>5.138432446995744</v>
       </c>
       <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
         <v>600</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>0</v>
       </c>
-      <c r="H18" t="n">
-        <v>29.70815987088802</v>
+      <c r="I18" t="n">
+        <v>21.94228754762253</v>
       </c>
     </row>
     <row r="19">
@@ -857,22 +913,25 @@
         <v>43833.33333333334</v>
       </c>
       <c r="C19" t="n">
-        <v>27.83240970094889</v>
+        <v>21.03589629771315</v>
       </c>
       <c r="D19" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>4.40357114650881</v>
+        <v>2.848353072482905</v>
       </c>
       <c r="F19" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H19" t="n">
-        <v>29.19998555791527</v>
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>21.32713225443267</v>
       </c>
     </row>
     <row r="20">
@@ -883,22 +942,25 @@
         <v>43833.41666666666</v>
       </c>
       <c r="C20" t="n">
-        <v>38.11229819827276</v>
+        <v>17.75088764351671</v>
       </c>
       <c r="D20" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>7.437633487287167</v>
+        <v>5.056873322027672</v>
       </c>
       <c r="F20" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H20" t="n">
-        <v>45.75600796120849</v>
+        <v>2</v>
+      </c>
+      <c r="I20" t="n">
+        <v>22.6061928555867</v>
       </c>
     </row>
     <row r="21">
@@ -909,22 +971,25 @@
         <v>43833.5</v>
       </c>
       <c r="C21" t="n">
-        <v>25.2660566787197</v>
+        <v>36.65519375467537</v>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E21" t="n">
-        <v>5.498796109779237</v>
+        <v>3.250034089064255</v>
       </c>
       <c r="F21" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H21" t="n">
-        <v>26.72206189264629</v>
+        <v>3</v>
+      </c>
+      <c r="I21" t="n">
+        <v>36.33332739512077</v>
       </c>
     </row>
     <row r="22">
@@ -935,22 +1000,25 @@
         <v>43833.58333333334</v>
       </c>
       <c r="C22" t="n">
-        <v>17.43604847354246</v>
+        <v>17.23247173360915</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>6.302864176385164</v>
+        <v>4.113995096738889</v>
       </c>
       <c r="F22" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G22" t="n">
+        <v>120</v>
+      </c>
+      <c r="H22" t="n">
         <v>4</v>
       </c>
-      <c r="H22" t="n">
-        <v>22.90067303590984</v>
+      <c r="I22" t="n">
+        <v>15.98930212592019</v>
       </c>
     </row>
     <row r="23">
@@ -961,22 +1029,25 @@
         <v>43833.66666666666</v>
       </c>
       <c r="C23" t="n">
-        <v>20.83794787483202</v>
+        <v>20.57306091068566</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E23" t="n">
-        <v>4.454612476247981</v>
+        <v>8.029310519916772</v>
       </c>
       <c r="F23" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G23" t="n">
+        <v>120</v>
+      </c>
+      <c r="H23" t="n">
         <v>5</v>
       </c>
-      <c r="H23" t="n">
-        <v>22.26234470207251</v>
+      <c r="I23" t="n">
+        <v>15.7394776086143</v>
       </c>
     </row>
     <row r="24">
@@ -987,22 +1058,25 @@
         <v>43833.75</v>
       </c>
       <c r="C24" t="n">
-        <v>24.29801601108552</v>
+        <v>20.35717574270336</v>
       </c>
       <c r="D24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E24" t="n">
-        <v>6.252314815436285</v>
+        <v>3.65903064290357</v>
       </c>
       <c r="F24" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G24" t="n">
+        <v>120</v>
+      </c>
+      <c r="H24" t="n">
         <v>6</v>
       </c>
-      <c r="H24" t="n">
-        <v>31.34767067259892</v>
+      <c r="I24" t="n">
+        <v>28.86806510638662</v>
       </c>
     </row>
     <row r="25">
@@ -1013,22 +1087,25 @@
         <v>43833.83333333334</v>
       </c>
       <c r="C25" t="n">
-        <v>38.36095861549008</v>
+        <v>18.5590324988497</v>
       </c>
       <c r="D25" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E25" t="n">
-        <v>6.601537355361818</v>
+        <v>2.7339721529473</v>
       </c>
       <c r="F25" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G25" t="n">
+        <v>120</v>
+      </c>
+      <c r="H25" t="n">
         <v>7</v>
       </c>
-      <c r="H25" t="n">
-        <v>30.76113767080232</v>
+      <c r="I25" t="n">
+        <v>15.70301184260797</v>
       </c>
     </row>
     <row r="26">
@@ -1039,22 +1116,25 @@
         <v>43834.25</v>
       </c>
       <c r="C26" t="n">
-        <v>36.19818554006719</v>
+        <v>30.36692873509379</v>
       </c>
       <c r="D26" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E26" t="n">
-        <v>6.520934028062626</v>
+        <v>3.489131942093357</v>
       </c>
       <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
         <v>600</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>0</v>
       </c>
-      <c r="H26" t="n">
-        <v>42.04308118408736</v>
+      <c r="I26" t="n">
+        <v>33.01579648943326</v>
       </c>
     </row>
     <row r="27">
@@ -1065,22 +1145,25 @@
         <v>43834.33333333334</v>
       </c>
       <c r="C27" t="n">
-        <v>38.34503881240138</v>
+        <v>20.91025224773324</v>
       </c>
       <c r="D27" t="n">
         <v>4</v>
       </c>
       <c r="E27" t="n">
-        <v>3.218637286081526</v>
+        <v>6.124670696028345</v>
       </c>
       <c r="F27" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H27" t="n">
-        <v>36.01577027439431</v>
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>17.54244116097739</v>
       </c>
     </row>
     <row r="28">
@@ -1091,22 +1174,25 @@
         <v>43834.41666666666</v>
       </c>
       <c r="C28" t="n">
-        <v>17.13388174006683</v>
+        <v>29.15656548549059</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2.877044824416498</v>
+        <v>8.676978938689125</v>
       </c>
       <c r="F28" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H28" t="n">
-        <v>20.18526151242939</v>
+        <v>2</v>
+      </c>
+      <c r="I28" t="n">
+        <v>24.43237732397563</v>
       </c>
     </row>
     <row r="29">
@@ -1117,22 +1203,25 @@
         <v>43834.5</v>
       </c>
       <c r="C29" t="n">
-        <v>24.10184114944363</v>
+        <v>16.58065637127932</v>
       </c>
       <c r="D29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" t="n">
-        <v>8.558276233578923</v>
+        <v>2.797462202890102</v>
       </c>
       <c r="F29" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G29" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H29" t="n">
-        <v>30.65885089160475</v>
+        <v>3</v>
+      </c>
+      <c r="I29" t="n">
+        <v>17.03427684793569</v>
       </c>
     </row>
     <row r="30">
@@ -1143,22 +1232,25 @@
         <v>43834.58333333334</v>
       </c>
       <c r="C30" t="n">
-        <v>33.02192280661066</v>
+        <v>23.54176976466573</v>
       </c>
       <c r="D30" t="n">
+        <v>10</v>
+      </c>
+      <c r="E30" t="n">
+        <v>8.669497060205929</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" t="n">
+        <v>120</v>
+      </c>
+      <c r="H30" t="n">
         <v>4</v>
       </c>
-      <c r="E30" t="n">
-        <v>9.810490684830343</v>
-      </c>
-      <c r="F30" t="n">
-        <v>120</v>
-      </c>
-      <c r="G30" t="n">
-        <v>4</v>
-      </c>
-      <c r="H30" t="n">
-        <v>35.85575286763583</v>
+      <c r="I30" t="n">
+        <v>22.9446188703026</v>
       </c>
     </row>
     <row r="31">
@@ -1169,22 +1261,25 @@
         <v>43834.66666666666</v>
       </c>
       <c r="C31" t="n">
-        <v>22.25694517076942</v>
+        <v>20.06184714949713</v>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E31" t="n">
-        <v>4.156305452044603</v>
+        <v>3.172144219901542</v>
       </c>
       <c r="F31" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
+        <v>120</v>
+      </c>
+      <c r="H31" t="n">
         <v>5</v>
       </c>
-      <c r="H31" t="n">
-        <v>20.03869444492405</v>
+      <c r="I31" t="n">
+        <v>15.97891679470175</v>
       </c>
     </row>
     <row r="32">
@@ -1195,22 +1290,25 @@
         <v>43834.75</v>
       </c>
       <c r="C32" t="n">
-        <v>25.85190267207324</v>
+        <v>37.53083439853464</v>
       </c>
       <c r="D32" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E32" t="n">
-        <v>6.18473984357264</v>
+        <v>6.973729838660874</v>
       </c>
       <c r="F32" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G32" t="n">
+        <v>120</v>
+      </c>
+      <c r="H32" t="n">
         <v>6</v>
       </c>
-      <c r="H32" t="n">
-        <v>25.02825846234123</v>
+      <c r="I32" t="n">
+        <v>38.66228218755853</v>
       </c>
     </row>
     <row r="33">
@@ -1221,22 +1319,25 @@
         <v>43834.83333333334</v>
       </c>
       <c r="C33" t="n">
-        <v>39.25296496806806</v>
+        <v>25.73299639159404</v>
       </c>
       <c r="D33" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E33" t="n">
-        <v>9.516955941762724</v>
+        <v>7.387969593677008</v>
       </c>
       <c r="F33" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G33" t="n">
+        <v>120</v>
+      </c>
+      <c r="H33" t="n">
         <v>7</v>
       </c>
-      <c r="H33" t="n">
-        <v>39.41954899164657</v>
+      <c r="I33" t="n">
+        <v>22.61567255036451</v>
       </c>
     </row>
     <row r="34">
@@ -1247,22 +1348,25 @@
         <v>43835.25</v>
       </c>
       <c r="C34" t="n">
-        <v>33.0213816472537</v>
+        <v>25.52345777535096</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" t="n">
-        <v>5.795391155412323</v>
+        <v>6.187695440700514</v>
       </c>
       <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
         <v>600</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>0</v>
       </c>
-      <c r="H34" t="n">
-        <v>36.29899036111942</v>
+      <c r="I34" t="n">
+        <v>29.4375900574336</v>
       </c>
     </row>
     <row r="35">
@@ -1273,22 +1377,25 @@
         <v>43835.33333333334</v>
       </c>
       <c r="C35" t="n">
-        <v>28.72489341432147</v>
+        <v>22.13972947809899</v>
       </c>
       <c r="D35" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E35" t="n">
-        <v>4.581413071379796</v>
+        <v>8.330261003057384</v>
       </c>
       <c r="F35" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H35" t="n">
-        <v>35.86159370940091</v>
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>33.31248370922215</v>
       </c>
     </row>
     <row r="36">
@@ -1299,22 +1406,25 @@
         <v>43835.41666666666</v>
       </c>
       <c r="C36" t="n">
-        <v>30.62426057087166</v>
+        <v>29.58241595939187</v>
       </c>
       <c r="D36" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E36" t="n">
-        <v>2.012496717249081</v>
+        <v>7.002431034967556</v>
       </c>
       <c r="F36" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H36" t="n">
-        <v>26.95734835816771</v>
+        <v>2</v>
+      </c>
+      <c r="I36" t="n">
+        <v>25.63980983464768</v>
       </c>
     </row>
     <row r="37">
@@ -1325,22 +1435,25 @@
         <v>43835.5</v>
       </c>
       <c r="C37" t="n">
-        <v>37.17074916904534</v>
+        <v>36.31603445605869</v>
       </c>
       <c r="D37" t="n">
         <v>12</v>
       </c>
       <c r="E37" t="n">
-        <v>7.466757769410377</v>
+        <v>3.031040891672776</v>
       </c>
       <c r="F37" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G37" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H37" t="n">
-        <v>39.27373266368544</v>
+        <v>3</v>
+      </c>
+      <c r="I37" t="n">
+        <v>39.12712166953845</v>
       </c>
     </row>
     <row r="38">
@@ -1351,22 +1464,25 @@
         <v>43835.58333333334</v>
       </c>
       <c r="C38" t="n">
-        <v>20.07763485407833</v>
+        <v>16.94761547987649</v>
       </c>
       <c r="D38" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E38" t="n">
-        <v>5.629762932730541</v>
+        <v>7.982696421531664</v>
       </c>
       <c r="F38" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G38" t="n">
+        <v>120</v>
+      </c>
+      <c r="H38" t="n">
         <v>4</v>
       </c>
-      <c r="H38" t="n">
-        <v>18.44796509767713</v>
+      <c r="I38" t="n">
+        <v>18.44843065692635</v>
       </c>
     </row>
     <row r="39">
@@ -1377,22 +1493,25 @@
         <v>43835.66666666666</v>
       </c>
       <c r="C39" t="n">
-        <v>31.87776962678478</v>
+        <v>31.64674529523073</v>
       </c>
       <c r="D39" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E39" t="n">
-        <v>8.505723395775746</v>
+        <v>5.40783940075357</v>
       </c>
       <c r="F39" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G39" t="n">
+        <v>120</v>
+      </c>
+      <c r="H39" t="n">
         <v>5</v>
       </c>
-      <c r="H39" t="n">
-        <v>33.91485560501488</v>
+      <c r="I39" t="n">
+        <v>32.86455903447688</v>
       </c>
     </row>
     <row r="40">
@@ -1403,22 +1522,25 @@
         <v>43835.75</v>
       </c>
       <c r="C40" t="n">
-        <v>31.35417849883929</v>
+        <v>17.26240597296849</v>
       </c>
       <c r="D40" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E40" t="n">
-        <v>8.088503051554511</v>
+        <v>9.711520431376613</v>
       </c>
       <c r="F40" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G40" t="n">
+        <v>120</v>
+      </c>
+      <c r="H40" t="n">
         <v>6</v>
       </c>
-      <c r="H40" t="n">
-        <v>31.42836381222881</v>
+      <c r="I40" t="n">
+        <v>14.04590173081479</v>
       </c>
     </row>
     <row r="41">
@@ -1429,22 +1551,25 @@
         <v>43835.83333333334</v>
       </c>
       <c r="C41" t="n">
-        <v>31.25641030863088</v>
+        <v>22.2042293089407</v>
       </c>
       <c r="D41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E41" t="n">
-        <v>9.574529575709278</v>
+        <v>4.561513346717843</v>
       </c>
       <c r="F41" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G41" t="n">
+        <v>120</v>
+      </c>
+      <c r="H41" t="n">
         <v>7</v>
       </c>
-      <c r="H41" t="n">
-        <v>30.48741534301278</v>
+      <c r="I41" t="n">
+        <v>19.07665650157256</v>
       </c>
     </row>
     <row r="42">
@@ -1455,22 +1580,25 @@
         <v>43836.25</v>
       </c>
       <c r="C42" t="n">
-        <v>33.57964575232252</v>
+        <v>33.14065736714303</v>
       </c>
       <c r="D42" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E42" t="n">
-        <v>3.152498969270306</v>
+        <v>5.357651267369174</v>
       </c>
       <c r="F42" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" t="n">
         <v>600</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>0</v>
       </c>
-      <c r="H42" t="n">
-        <v>41.01706756388896</v>
+      <c r="I42" t="n">
+        <v>38.89415521473416</v>
       </c>
     </row>
     <row r="43">
@@ -1481,22 +1609,25 @@
         <v>43836.33333333334</v>
       </c>
       <c r="C43" t="n">
-        <v>39.3641212296111</v>
+        <v>16.01033925592656</v>
       </c>
       <c r="D43" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>5.460283867209626</v>
+        <v>6.830229572513998</v>
       </c>
       <c r="F43" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H43" t="n">
-        <v>40.24893377565023</v>
+        <v>1</v>
+      </c>
+      <c r="I43" t="n">
+        <v>18.66801219706832</v>
       </c>
     </row>
     <row r="44">
@@ -1507,22 +1638,25 @@
         <v>43836.41666666666</v>
       </c>
       <c r="C44" t="n">
-        <v>20.04927023198717</v>
+        <v>24.85578325019149</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5.189231717417353</v>
+        <v>4.702151292693562</v>
       </c>
       <c r="F44" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H44" t="n">
-        <v>21.54357267802881</v>
+        <v>2</v>
+      </c>
+      <c r="I44" t="n">
+        <v>25.17203929771168</v>
       </c>
     </row>
     <row r="45">
@@ -1533,22 +1667,25 @@
         <v>43836.5</v>
       </c>
       <c r="C45" t="n">
-        <v>29.54120302588742</v>
+        <v>26.85402428715196</v>
       </c>
       <c r="D45" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E45" t="n">
-        <v>8.944414469876829</v>
+        <v>6.57824667586821</v>
       </c>
       <c r="F45" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G45" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H45" t="n">
-        <v>28.95740014513866</v>
+        <v>3</v>
+      </c>
+      <c r="I45" t="n">
+        <v>25.55042118584958</v>
       </c>
     </row>
     <row r="46">
@@ -1559,22 +1696,25 @@
         <v>43836.58333333334</v>
       </c>
       <c r="C46" t="n">
-        <v>23.95310495179412</v>
+        <v>30.53355972307873</v>
       </c>
       <c r="D46" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3.937335441831849</v>
+        <v>5.074269407791367</v>
       </c>
       <c r="F46" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G46" t="n">
+        <v>120</v>
+      </c>
+      <c r="H46" t="n">
         <v>4</v>
       </c>
-      <c r="H46" t="n">
-        <v>29.29627960331221</v>
+      <c r="I46" t="n">
+        <v>28.43281906738631</v>
       </c>
     </row>
     <row r="47">
@@ -1585,22 +1725,25 @@
         <v>43836.66666666666</v>
       </c>
       <c r="C47" t="n">
-        <v>17.52612964479626</v>
+        <v>20.72564254426629</v>
       </c>
       <c r="D47" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E47" t="n">
-        <v>7.737856336760105</v>
+        <v>6.273593281046394</v>
       </c>
       <c r="F47" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G47" t="n">
+        <v>120</v>
+      </c>
+      <c r="H47" t="n">
         <v>5</v>
       </c>
-      <c r="H47" t="n">
-        <v>12.16699617109783</v>
+      <c r="I47" t="n">
+        <v>28.2498726257494</v>
       </c>
     </row>
     <row r="48">
@@ -1611,22 +1754,25 @@
         <v>43836.75</v>
       </c>
       <c r="C48" t="n">
-        <v>29.99725105931248</v>
+        <v>16.99416362454907</v>
       </c>
       <c r="D48" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>6.351130182282307</v>
+        <v>9.277645800289115</v>
       </c>
       <c r="F48" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G48" t="n">
+        <v>120</v>
+      </c>
+      <c r="H48" t="n">
         <v>6</v>
       </c>
-      <c r="H48" t="n">
-        <v>32.29911982556375</v>
+      <c r="I48" t="n">
+        <v>14.17713279903975</v>
       </c>
     </row>
     <row r="49">
@@ -1637,22 +1783,25 @@
         <v>43836.83333333334</v>
       </c>
       <c r="C49" t="n">
-        <v>25.68784813205218</v>
+        <v>17.16179394476993</v>
       </c>
       <c r="D49" t="n">
         <v>6</v>
       </c>
       <c r="E49" t="n">
-        <v>8.465649531260445</v>
+        <v>2.89034326454222</v>
       </c>
       <c r="F49" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G49" t="n">
+        <v>120</v>
+      </c>
+      <c r="H49" t="n">
         <v>7</v>
       </c>
-      <c r="H49" t="n">
-        <v>30.40826241767484</v>
+      <c r="I49" t="n">
+        <v>12.97104075647256</v>
       </c>
     </row>
     <row r="50">
@@ -1663,22 +1812,25 @@
         <v>43837.25</v>
       </c>
       <c r="C50" t="n">
-        <v>37.32957555046254</v>
+        <v>35.60233814021228</v>
       </c>
       <c r="D50" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E50" t="n">
-        <v>9.504046869646093</v>
+        <v>8.762958622098244</v>
       </c>
       <c r="F50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" t="n">
         <v>600</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>0</v>
       </c>
-      <c r="H50" t="n">
-        <v>37.68737424994553</v>
+      <c r="I50" t="n">
+        <v>37.21564549465322</v>
       </c>
     </row>
     <row r="51">
@@ -1689,22 +1841,25 @@
         <v>43837.33333333334</v>
       </c>
       <c r="C51" t="n">
-        <v>35.61194315128305</v>
+        <v>19.65825027620401</v>
       </c>
       <c r="D51" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E51" t="n">
-        <v>4.870839208401197</v>
+        <v>7.954460902888642</v>
       </c>
       <c r="F51" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H51" t="n">
-        <v>37.84950331920304</v>
+        <v>1</v>
+      </c>
+      <c r="I51" t="n">
+        <v>18.46460448999101</v>
       </c>
     </row>
     <row r="52">
@@ -1715,22 +1870,25 @@
         <v>43837.41666666666</v>
       </c>
       <c r="C52" t="n">
-        <v>31.28533591752803</v>
+        <v>39.59390811272051</v>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E52" t="n">
-        <v>6.156208041543812</v>
+        <v>5.183986407832453</v>
       </c>
       <c r="F52" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H52" t="n">
-        <v>32.17253896007256</v>
+        <v>2</v>
+      </c>
+      <c r="I52" t="n">
+        <v>40.9456991934917</v>
       </c>
     </row>
     <row r="53">
@@ -1741,22 +1899,25 @@
         <v>43837.5</v>
       </c>
       <c r="C53" t="n">
-        <v>26.75881209465732</v>
+        <v>20.22630446503938</v>
       </c>
       <c r="D53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E53" t="n">
-        <v>6.675117021982787</v>
+        <v>3.441803116798488</v>
       </c>
       <c r="F53" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G53" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H53" t="n">
-        <v>32.02091220884321</v>
+        <v>3</v>
+      </c>
+      <c r="I53" t="n">
+        <v>18.36474812576084</v>
       </c>
     </row>
     <row r="54">
@@ -1767,22 +1928,25 @@
         <v>43837.58333333334</v>
       </c>
       <c r="C54" t="n">
-        <v>19.48459363466588</v>
+        <v>26.28921493507695</v>
       </c>
       <c r="D54" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E54" t="n">
-        <v>3.937892531620971</v>
+        <v>5.66719022968597</v>
       </c>
       <c r="F54" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G54" t="n">
+        <v>120</v>
+      </c>
+      <c r="H54" t="n">
         <v>4</v>
       </c>
-      <c r="H54" t="n">
-        <v>18.79360986224458</v>
+      <c r="I54" t="n">
+        <v>20.94754183381712</v>
       </c>
     </row>
     <row r="55">
@@ -1793,22 +1957,25 @@
         <v>43837.66666666666</v>
       </c>
       <c r="C55" t="n">
-        <v>17.53970852950311</v>
+        <v>15.66066590075732</v>
       </c>
       <c r="D55" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E55" t="n">
-        <v>4.09424139916527</v>
+        <v>5.06759056218073</v>
       </c>
       <c r="F55" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G55" t="n">
+        <v>120</v>
+      </c>
+      <c r="H55" t="n">
         <v>5</v>
       </c>
-      <c r="H55" t="n">
-        <v>22.05136321593109</v>
+      <c r="I55" t="n">
+        <v>18.90640318535507</v>
       </c>
     </row>
     <row r="56">
@@ -1819,22 +1986,25 @@
         <v>43837.75</v>
       </c>
       <c r="C56" t="n">
-        <v>27.13324377710932</v>
+        <v>32.62370295385168</v>
       </c>
       <c r="D56" t="n">
         <v>11</v>
       </c>
       <c r="E56" t="n">
-        <v>4.723126737601727</v>
+        <v>9.643298374204548</v>
       </c>
       <c r="F56" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G56" t="n">
+        <v>120</v>
+      </c>
+      <c r="H56" t="n">
         <v>6</v>
       </c>
-      <c r="H56" t="n">
-        <v>20.32920676134363</v>
+      <c r="I56" t="n">
+        <v>36.6598821448405</v>
       </c>
     </row>
     <row r="57">
@@ -1845,22 +2015,25 @@
         <v>43837.83333333334</v>
       </c>
       <c r="C57" t="n">
-        <v>17.09154925632101</v>
+        <v>34.3394544830301</v>
       </c>
       <c r="D57" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E57" t="n">
-        <v>6.083671635439791</v>
+        <v>9.941998753198085</v>
       </c>
       <c r="F57" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G57" t="n">
+        <v>120</v>
+      </c>
+      <c r="H57" t="n">
         <v>7</v>
       </c>
-      <c r="H57" t="n">
-        <v>13.97820907735203</v>
+      <c r="I57" t="n">
+        <v>34.3818129055884</v>
       </c>
     </row>
     <row r="58">
@@ -1871,22 +2044,25 @@
         <v>43838.25</v>
       </c>
       <c r="C58" t="n">
-        <v>23.46389243131839</v>
+        <v>36.83942517507172</v>
       </c>
       <c r="D58" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7.521116999176572</v>
+        <v>2.346836541300276</v>
       </c>
       <c r="F58" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" t="n">
         <v>600</v>
       </c>
-      <c r="G58" t="n">
+      <c r="H58" t="n">
         <v>0</v>
       </c>
-      <c r="H58" t="n">
-        <v>25.45119830891657</v>
+      <c r="I58" t="n">
+        <v>37.51119504689286</v>
       </c>
     </row>
     <row r="59">
@@ -1897,22 +2073,25 @@
         <v>43838.33333333334</v>
       </c>
       <c r="C59" t="n">
-        <v>20.69294053110106</v>
+        <v>19.12057733891297</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E59" t="n">
-        <v>9.957730220200975</v>
+        <v>2.216163876262614</v>
       </c>
       <c r="F59" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G59" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H59" t="n">
-        <v>22.32373267087669</v>
+        <v>1</v>
+      </c>
+      <c r="I59" t="n">
+        <v>21.17903428627698</v>
       </c>
     </row>
     <row r="60">
@@ -1923,22 +2102,25 @@
         <v>43838.41666666666</v>
       </c>
       <c r="C60" t="n">
-        <v>24.56482979391903</v>
+        <v>27.46291550241618</v>
       </c>
       <c r="D60" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E60" t="n">
-        <v>9.641268938631796</v>
+        <v>7.892904761078023</v>
       </c>
       <c r="F60" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G60" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H60" t="n">
-        <v>20.61278294791001</v>
+        <v>2</v>
+      </c>
+      <c r="I60" t="n">
+        <v>25.65878719281995</v>
       </c>
     </row>
     <row r="61">
@@ -1949,22 +2131,25 @@
         <v>43838.5</v>
       </c>
       <c r="C61" t="n">
-        <v>24.00182333601692</v>
+        <v>25.03322975255617</v>
       </c>
       <c r="D61" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E61" t="n">
-        <v>4.247909661345482</v>
+        <v>7.963094783723406</v>
       </c>
       <c r="F61" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G61" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H61" t="n">
-        <v>24.36544603228566</v>
+        <v>3</v>
+      </c>
+      <c r="I61" t="n">
+        <v>23.09966851741985</v>
       </c>
     </row>
     <row r="62">
@@ -1975,22 +2160,25 @@
         <v>43838.58333333334</v>
       </c>
       <c r="C62" t="n">
-        <v>27.00387570934957</v>
+        <v>29.7988736873935</v>
       </c>
       <c r="D62" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E62" t="n">
-        <v>5.179307455877139</v>
+        <v>2.451308394849942</v>
       </c>
       <c r="F62" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G62" t="n">
+        <v>120</v>
+      </c>
+      <c r="H62" t="n">
         <v>4</v>
       </c>
-      <c r="H62" t="n">
-        <v>28.59801706358018</v>
+      <c r="I62" t="n">
+        <v>22.51389304623652</v>
       </c>
     </row>
     <row r="63">
@@ -2001,22 +2189,25 @@
         <v>43838.66666666666</v>
       </c>
       <c r="C63" t="n">
-        <v>39.09056641380155</v>
+        <v>36.0534102839933</v>
       </c>
       <c r="D63" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E63" t="n">
-        <v>4.585208821820545</v>
+        <v>3.784189068328127</v>
       </c>
       <c r="F63" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G63" t="n">
+        <v>120</v>
+      </c>
+      <c r="H63" t="n">
         <v>5</v>
       </c>
-      <c r="H63" t="n">
-        <v>38.69028461262006</v>
+      <c r="I63" t="n">
+        <v>42.0247893572218</v>
       </c>
     </row>
     <row r="64">
@@ -2027,22 +2218,25 @@
         <v>43838.75</v>
       </c>
       <c r="C64" t="n">
-        <v>31.59193053365035</v>
+        <v>30.92056662346785</v>
       </c>
       <c r="D64" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E64" t="n">
-        <v>7.14281320148308</v>
+        <v>6.380815294069901</v>
       </c>
       <c r="F64" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G64" t="n">
+        <v>120</v>
+      </c>
+      <c r="H64" t="n">
         <v>6</v>
       </c>
-      <c r="H64" t="n">
-        <v>25.94231912182622</v>
+      <c r="I64" t="n">
+        <v>38.65610847568296</v>
       </c>
     </row>
     <row r="65">
@@ -2053,22 +2247,25 @@
         <v>43838.83333333334</v>
       </c>
       <c r="C65" t="n">
-        <v>32.42104688685303</v>
+        <v>18.24238846251783</v>
       </c>
       <c r="D65" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E65" t="n">
-        <v>6.058407755315959</v>
+        <v>2.671934226056107</v>
       </c>
       <c r="F65" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G65" t="n">
+        <v>120</v>
+      </c>
+      <c r="H65" t="n">
         <v>7</v>
       </c>
-      <c r="H65" t="n">
-        <v>30.91435751793391</v>
+      <c r="I65" t="n">
+        <v>17.25041906399691</v>
       </c>
     </row>
     <row r="66">
@@ -2079,22 +2276,25 @@
         <v>43839.25</v>
       </c>
       <c r="C66" t="n">
-        <v>31.00750349368803</v>
+        <v>33.7793017559883</v>
       </c>
       <c r="D66" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E66" t="n">
-        <v>7.137684530337697</v>
+        <v>3.97034186344281</v>
       </c>
       <c r="F66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" t="n">
         <v>600</v>
       </c>
-      <c r="G66" t="n">
+      <c r="H66" t="n">
         <v>0</v>
       </c>
-      <c r="H66" t="n">
-        <v>27.86539448339329</v>
+      <c r="I66" t="n">
+        <v>29.80267543359637</v>
       </c>
     </row>
     <row r="67">
@@ -2105,22 +2305,25 @@
         <v>43839.33333333334</v>
       </c>
       <c r="C67" t="n">
-        <v>37.74492647307432</v>
+        <v>38.04494008987099</v>
       </c>
       <c r="D67" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E67" t="n">
-        <v>7.940620056526708</v>
+        <v>4.333801785488944</v>
       </c>
       <c r="F67" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H67" t="n">
-        <v>43.9945547393913</v>
+        <v>1</v>
+      </c>
+      <c r="I67" t="n">
+        <v>39.20445813707417</v>
       </c>
     </row>
     <row r="68">
@@ -2131,22 +2334,25 @@
         <v>43839.41666666666</v>
       </c>
       <c r="C68" t="n">
-        <v>22.53744905749768</v>
+        <v>39.48091362289944</v>
       </c>
       <c r="D68" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E68" t="n">
-        <v>8.128360492075169</v>
+        <v>3.994830556152307</v>
       </c>
       <c r="F68" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G68" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H68" t="n">
-        <v>26.20706399743539</v>
+        <v>2</v>
+      </c>
+      <c r="I68" t="n">
+        <v>32.1349655149376</v>
       </c>
     </row>
     <row r="69">
@@ -2157,22 +2363,25 @@
         <v>43839.5</v>
       </c>
       <c r="C69" t="n">
-        <v>33.98233990900512</v>
+        <v>15.74885703615104</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E69" t="n">
-        <v>2.104434164403027</v>
+        <v>8.251469732131341</v>
       </c>
       <c r="F69" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G69" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H69" t="n">
-        <v>35.92058940568235</v>
+        <v>3</v>
+      </c>
+      <c r="I69" t="n">
+        <v>14.783529857663</v>
       </c>
     </row>
     <row r="70">
@@ -2183,22 +2392,25 @@
         <v>43839.58333333334</v>
       </c>
       <c r="C70" t="n">
-        <v>24.41110964795081</v>
+        <v>38.7087877947347</v>
       </c>
       <c r="D70" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E70" t="n">
-        <v>9.508224090762791</v>
+        <v>2.57689267345827</v>
       </c>
       <c r="F70" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G70" t="n">
+        <v>120</v>
+      </c>
+      <c r="H70" t="n">
         <v>4</v>
       </c>
-      <c r="H70" t="n">
-        <v>22.06044464563608</v>
+      <c r="I70" t="n">
+        <v>38.02229893050355</v>
       </c>
     </row>
     <row r="71">
@@ -2209,22 +2421,25 @@
         <v>43839.66666666666</v>
       </c>
       <c r="C71" t="n">
-        <v>19.27067211603622</v>
+        <v>32.5089675305922</v>
       </c>
       <c r="D71" t="n">
+        <v>3</v>
+      </c>
+      <c r="E71" t="n">
+        <v>8.163458603404472</v>
+      </c>
+      <c r="F71" t="n">
+        <v>2</v>
+      </c>
+      <c r="G71" t="n">
+        <v>120</v>
+      </c>
+      <c r="H71" t="n">
         <v>5</v>
       </c>
-      <c r="E71" t="n">
-        <v>5.310507011515099</v>
-      </c>
-      <c r="F71" t="n">
-        <v>120</v>
-      </c>
-      <c r="G71" t="n">
-        <v>5</v>
-      </c>
-      <c r="H71" t="n">
-        <v>15.03753609417123</v>
+      <c r="I71" t="n">
+        <v>30.65683412751963</v>
       </c>
     </row>
     <row r="72">
@@ -2235,22 +2450,25 @@
         <v>43839.75</v>
       </c>
       <c r="C72" t="n">
-        <v>31.71315575209378</v>
+        <v>37.19369719017957</v>
       </c>
       <c r="D72" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E72" t="n">
-        <v>3.683176114225918</v>
+        <v>8.786862633701276</v>
       </c>
       <c r="F72" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G72" t="n">
+        <v>120</v>
+      </c>
+      <c r="H72" t="n">
         <v>6</v>
       </c>
-      <c r="H72" t="n">
-        <v>32.32116789360875</v>
+      <c r="I72" t="n">
+        <v>33.2211949927663</v>
       </c>
     </row>
     <row r="73">
@@ -2261,22 +2479,25 @@
         <v>43839.83333333334</v>
       </c>
       <c r="C73" t="n">
-        <v>24.34649566250796</v>
+        <v>18.62942387555943</v>
       </c>
       <c r="D73" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E73" t="n">
-        <v>6.189802727203507</v>
+        <v>3.519584491977069</v>
       </c>
       <c r="F73" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G73" t="n">
+        <v>120</v>
+      </c>
+      <c r="H73" t="n">
         <v>7</v>
       </c>
-      <c r="H73" t="n">
-        <v>22.96749868548693</v>
+      <c r="I73" t="n">
+        <v>19.70489145483246</v>
       </c>
     </row>
     <row r="74">
@@ -2287,22 +2508,25 @@
         <v>43840.25</v>
       </c>
       <c r="C74" t="n">
-        <v>27.16931265310011</v>
+        <v>29.4940768562953</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E74" t="n">
-        <v>5.592682775927773</v>
+        <v>2.519722396322179</v>
       </c>
       <c r="F74" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" t="n">
         <v>600</v>
       </c>
-      <c r="G74" t="n">
+      <c r="H74" t="n">
         <v>0</v>
       </c>
-      <c r="H74" t="n">
-        <v>28.75697062515496</v>
+      <c r="I74" t="n">
+        <v>31.95332019577055</v>
       </c>
     </row>
     <row r="75">
@@ -2313,22 +2537,25 @@
         <v>43840.33333333334</v>
       </c>
       <c r="C75" t="n">
-        <v>38.07665230571689</v>
+        <v>25.30779417037781</v>
       </c>
       <c r="D75" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6.410160479203944</v>
+        <v>8.85124745516115</v>
       </c>
       <c r="F75" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G75" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H75" t="n">
-        <v>36.81995092131175</v>
+        <v>1</v>
+      </c>
+      <c r="I75" t="n">
+        <v>21.46199906180577</v>
       </c>
     </row>
     <row r="76">
@@ -2339,22 +2566,25 @@
         <v>43840.41666666666</v>
       </c>
       <c r="C76" t="n">
-        <v>31.43412142611029</v>
+        <v>24.58244791803756</v>
       </c>
       <c r="D76" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E76" t="n">
-        <v>6.962873467313777</v>
+        <v>9.083482954726687</v>
       </c>
       <c r="F76" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G76" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H76" t="n">
-        <v>33.41910779390086</v>
+        <v>2</v>
+      </c>
+      <c r="I76" t="n">
+        <v>18.6502339278611</v>
       </c>
     </row>
     <row r="77">
@@ -2365,22 +2595,25 @@
         <v>43840.5</v>
       </c>
       <c r="C77" t="n">
-        <v>19.81786147026024</v>
+        <v>28.77981922932279</v>
       </c>
       <c r="D77" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E77" t="n">
-        <v>8.190146675121008</v>
+        <v>5.39954031835035</v>
       </c>
       <c r="F77" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G77" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H77" t="n">
-        <v>19.27572530873701</v>
+        <v>3</v>
+      </c>
+      <c r="I77" t="n">
+        <v>27.79680183917325</v>
       </c>
     </row>
     <row r="78">
@@ -2391,22 +2624,25 @@
         <v>43840.58333333334</v>
       </c>
       <c r="C78" t="n">
-        <v>24.44001238616515</v>
+        <v>28.87827997760621</v>
       </c>
       <c r="D78" t="n">
         <v>6</v>
       </c>
       <c r="E78" t="n">
-        <v>7.011255041488102</v>
+        <v>2.423831961199533</v>
       </c>
       <c r="F78" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G78" t="n">
+        <v>120</v>
+      </c>
+      <c r="H78" t="n">
         <v>4</v>
       </c>
-      <c r="H78" t="n">
-        <v>23.20491264117859</v>
+      <c r="I78" t="n">
+        <v>26.23907406852805</v>
       </c>
     </row>
     <row r="79">
@@ -2417,22 +2653,25 @@
         <v>43840.66666666666</v>
       </c>
       <c r="C79" t="n">
-        <v>36.67859509091281</v>
+        <v>18.68753922475029</v>
       </c>
       <c r="D79" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E79" t="n">
-        <v>7.919071127439636</v>
+        <v>6.560379939832584</v>
       </c>
       <c r="F79" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G79" t="n">
+        <v>120</v>
+      </c>
+      <c r="H79" t="n">
         <v>5</v>
       </c>
-      <c r="H79" t="n">
-        <v>36.8072083653529</v>
+      <c r="I79" t="n">
+        <v>17.17149892048879</v>
       </c>
     </row>
     <row r="80">
@@ -2443,22 +2682,25 @@
         <v>43840.75</v>
       </c>
       <c r="C80" t="n">
-        <v>21.78373482764253</v>
+        <v>20.80665082656333</v>
       </c>
       <c r="D80" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E80" t="n">
-        <v>8.98243083723958</v>
+        <v>5.383584852810452</v>
       </c>
       <c r="F80" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G80" t="n">
+        <v>120</v>
+      </c>
+      <c r="H80" t="n">
         <v>6</v>
       </c>
-      <c r="H80" t="n">
-        <v>24.93971585920476</v>
+      <c r="I80" t="n">
+        <v>24.05138500559112</v>
       </c>
     </row>
     <row r="81">
@@ -2469,22 +2711,25 @@
         <v>43840.83333333334</v>
       </c>
       <c r="C81" t="n">
-        <v>30.03095356267747</v>
+        <v>18.89833498837527</v>
       </c>
       <c r="D81" t="n">
         <v>1</v>
       </c>
       <c r="E81" t="n">
-        <v>3.010846348318374</v>
+        <v>8.370388058576584</v>
       </c>
       <c r="F81" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G81" t="n">
+        <v>120</v>
+      </c>
+      <c r="H81" t="n">
         <v>7</v>
       </c>
-      <c r="H81" t="n">
-        <v>31.44862384094821</v>
+      <c r="I81" t="n">
+        <v>16.84807359260904</v>
       </c>
     </row>
     <row r="82">
@@ -2495,22 +2740,25 @@
         <v>43841.25</v>
       </c>
       <c r="C82" t="n">
-        <v>21.77384548975745</v>
+        <v>32.10008547205805</v>
       </c>
       <c r="D82" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E82" t="n">
-        <v>3.902792847093078</v>
+        <v>5.886051639938839</v>
       </c>
       <c r="F82" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" t="n">
         <v>600</v>
       </c>
-      <c r="G82" t="n">
+      <c r="H82" t="n">
         <v>0</v>
       </c>
-      <c r="H82" t="n">
-        <v>17.80687847106724</v>
+      <c r="I82" t="n">
+        <v>36.41361971932827</v>
       </c>
     </row>
     <row r="83">
@@ -2521,22 +2769,25 @@
         <v>43841.33333333334</v>
       </c>
       <c r="C83" t="n">
-        <v>18.35962016291351</v>
+        <v>17.8030893394303</v>
       </c>
       <c r="D83" t="n">
         <v>8</v>
       </c>
       <c r="E83" t="n">
-        <v>7.920561551224261</v>
+        <v>3.863715195971171</v>
       </c>
       <c r="F83" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H83" t="n">
-        <v>14.6357273016007</v>
+        <v>1</v>
+      </c>
+      <c r="I83" t="n">
+        <v>11.83213634539175</v>
       </c>
     </row>
     <row r="84">
@@ -2547,22 +2798,25 @@
         <v>43841.41666666666</v>
       </c>
       <c r="C84" t="n">
-        <v>20.85955437888591</v>
+        <v>18.13487510614519</v>
       </c>
       <c r="D84" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E84" t="n">
-        <v>9.662028678815844</v>
+        <v>9.255389568404635</v>
       </c>
       <c r="F84" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G84" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H84" t="n">
-        <v>25.7367637060697</v>
+        <v>2</v>
+      </c>
+      <c r="I84" t="n">
+        <v>24.10436331153892</v>
       </c>
     </row>
     <row r="85">
@@ -2573,22 +2827,25 @@
         <v>43841.5</v>
       </c>
       <c r="C85" t="n">
-        <v>37.69873936783588</v>
+        <v>22.38844236547895</v>
       </c>
       <c r="D85" t="n">
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7.858681058178584</v>
+        <v>5.815547672297999</v>
       </c>
       <c r="F85" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G85" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H85" t="n">
-        <v>40.24353354968554</v>
+        <v>3</v>
+      </c>
+      <c r="I85" t="n">
+        <v>18.60528517842334</v>
       </c>
     </row>
     <row r="86">
@@ -2599,22 +2856,25 @@
         <v>43841.58333333334</v>
       </c>
       <c r="C86" t="n">
-        <v>19.02300794825539</v>
+        <v>38.3009998626862</v>
       </c>
       <c r="D86" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E86" t="n">
-        <v>6.888401870454499</v>
+        <v>5.866138494935147</v>
       </c>
       <c r="F86" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G86" t="n">
+        <v>120</v>
+      </c>
+      <c r="H86" t="n">
         <v>4</v>
       </c>
-      <c r="H86" t="n">
-        <v>7.415851932857857</v>
+      <c r="I86" t="n">
+        <v>35.55063985988106</v>
       </c>
     </row>
     <row r="87">
@@ -2625,22 +2885,25 @@
         <v>43841.66666666666</v>
       </c>
       <c r="C87" t="n">
-        <v>32.16653007164955</v>
+        <v>33.0594879041539</v>
       </c>
       <c r="D87" t="n">
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>8.262533999725797</v>
+        <v>8.982254383276947</v>
       </c>
       <c r="F87" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G87" t="n">
+        <v>120</v>
+      </c>
+      <c r="H87" t="n">
         <v>5</v>
       </c>
-      <c r="H87" t="n">
-        <v>32.73362154934701</v>
+      <c r="I87" t="n">
+        <v>37.33538049575788</v>
       </c>
     </row>
     <row r="88">
@@ -2651,22 +2914,25 @@
         <v>43841.75</v>
       </c>
       <c r="C88" t="n">
-        <v>20.53757509130089</v>
+        <v>19.40011398303254</v>
       </c>
       <c r="D88" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E88" t="n">
-        <v>4.18948767565193</v>
+        <v>7.433703726056806</v>
       </c>
       <c r="F88" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G88" t="n">
+        <v>120</v>
+      </c>
+      <c r="H88" t="n">
         <v>6</v>
       </c>
-      <c r="H88" t="n">
-        <v>19.76716239179198</v>
+      <c r="I88" t="n">
+        <v>15.16040280733074</v>
       </c>
     </row>
     <row r="89">
@@ -2677,22 +2943,25 @@
         <v>43841.83333333334</v>
       </c>
       <c r="C89" t="n">
-        <v>36.35717382108251</v>
+        <v>27.40597724649921</v>
       </c>
       <c r="D89" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>9.1766904700387</v>
+        <v>3.739988805795743</v>
       </c>
       <c r="F89" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G89" t="n">
+        <v>120</v>
+      </c>
+      <c r="H89" t="n">
         <v>7</v>
       </c>
-      <c r="H89" t="n">
-        <v>25.87415365502084</v>
+      <c r="I89" t="n">
+        <v>24.01716783644229</v>
       </c>
     </row>
     <row r="90">
@@ -2703,22 +2972,25 @@
         <v>43842.25</v>
       </c>
       <c r="C90" t="n">
-        <v>26.05316411828704</v>
+        <v>30.69238501612093</v>
       </c>
       <c r="D90" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E90" t="n">
-        <v>3.481976852010483</v>
+        <v>6.306586113056521</v>
       </c>
       <c r="F90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G90" t="n">
         <v>600</v>
       </c>
-      <c r="G90" t="n">
+      <c r="H90" t="n">
         <v>0</v>
       </c>
-      <c r="H90" t="n">
-        <v>26.35400810528325</v>
+      <c r="I90" t="n">
+        <v>22.9853903924667</v>
       </c>
     </row>
     <row r="91">
@@ -2729,22 +3001,25 @@
         <v>43842.33333333334</v>
       </c>
       <c r="C91" t="n">
-        <v>36.87670505382991</v>
+        <v>36.75741992409105</v>
       </c>
       <c r="D91" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E91" t="n">
-        <v>5.757642199952085</v>
+        <v>2.267899817444692</v>
       </c>
       <c r="F91" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G91" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H91" t="n">
-        <v>33.22458509995188</v>
+        <v>1</v>
+      </c>
+      <c r="I91" t="n">
+        <v>35.597656365845</v>
       </c>
     </row>
     <row r="92">
@@ -2755,22 +3030,25 @@
         <v>43842.41666666666</v>
       </c>
       <c r="C92" t="n">
-        <v>20.94042414913468</v>
+        <v>17.39122293441421</v>
       </c>
       <c r="D92" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E92" t="n">
-        <v>3.720334059148334</v>
+        <v>4.689138952839311</v>
       </c>
       <c r="F92" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G92" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H92" t="n">
-        <v>17.12117862565076</v>
+        <v>2</v>
+      </c>
+      <c r="I92" t="n">
+        <v>17.74447091067043</v>
       </c>
     </row>
     <row r="93">
@@ -2781,22 +3059,25 @@
         <v>43842.5</v>
       </c>
       <c r="C93" t="n">
-        <v>37.85261188575335</v>
+        <v>17.67120797685015</v>
       </c>
       <c r="D93" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E93" t="n">
-        <v>9.997879160958725</v>
+        <v>5.618587299600671</v>
       </c>
       <c r="F93" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G93" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H93" t="n">
-        <v>35.41795800810243</v>
+        <v>3</v>
+      </c>
+      <c r="I93" t="n">
+        <v>15.59748758086319</v>
       </c>
     </row>
     <row r="94">
@@ -2807,22 +3088,25 @@
         <v>43842.58333333334</v>
       </c>
       <c r="C94" t="n">
-        <v>21.79189801284146</v>
+        <v>22.29402758810942</v>
       </c>
       <c r="D94" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E94" t="n">
-        <v>9.894612303078691</v>
+        <v>6.893542250609997</v>
       </c>
       <c r="F94" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G94" t="n">
+        <v>120</v>
+      </c>
+      <c r="H94" t="n">
         <v>4</v>
       </c>
-      <c r="H94" t="n">
-        <v>23.14968317593737</v>
+      <c r="I94" t="n">
+        <v>15.64452764269477</v>
       </c>
     </row>
     <row r="95">
@@ -2833,22 +3117,25 @@
         <v>43842.66666666666</v>
       </c>
       <c r="C95" t="n">
-        <v>24.38204346687255</v>
+        <v>24.2981240965844</v>
       </c>
       <c r="D95" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E95" t="n">
-        <v>3.400929628540738</v>
+        <v>7.748373367049134</v>
       </c>
       <c r="F95" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G95" t="n">
+        <v>120</v>
+      </c>
+      <c r="H95" t="n">
         <v>5</v>
       </c>
-      <c r="H95" t="n">
-        <v>26.45557015595883</v>
+      <c r="I95" t="n">
+        <v>26.54894487863574</v>
       </c>
     </row>
     <row r="96">
@@ -2859,22 +3146,25 @@
         <v>43842.75</v>
       </c>
       <c r="C96" t="n">
-        <v>20.30681978847973</v>
+        <v>26.25947278226883</v>
       </c>
       <c r="D96" t="n">
         <v>3</v>
       </c>
       <c r="E96" t="n">
-        <v>7.739136586145495</v>
+        <v>8.851881897022613</v>
       </c>
       <c r="F96" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G96" t="n">
+        <v>120</v>
+      </c>
+      <c r="H96" t="n">
         <v>6</v>
       </c>
-      <c r="H96" t="n">
-        <v>14.08253172938044</v>
+      <c r="I96" t="n">
+        <v>24.80959381837847</v>
       </c>
     </row>
     <row r="97">
@@ -2885,22 +3175,25 @@
         <v>43842.83333333334</v>
       </c>
       <c r="C97" t="n">
-        <v>30.0085064333453</v>
+        <v>33.35877051412669</v>
       </c>
       <c r="D97" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E97" t="n">
-        <v>7.062211523589793</v>
+        <v>7.658036388977922</v>
       </c>
       <c r="F97" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G97" t="n">
+        <v>120</v>
+      </c>
+      <c r="H97" t="n">
         <v>7</v>
       </c>
-      <c r="H97" t="n">
-        <v>26.07020598815859</v>
+      <c r="I97" t="n">
+        <v>36.59397434357545</v>
       </c>
     </row>
     <row r="98">
@@ -2911,22 +3204,25 @@
         <v>43843.25</v>
       </c>
       <c r="C98" t="n">
-        <v>17.70481768732204</v>
+        <v>21.69489100348198</v>
       </c>
       <c r="D98" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E98" t="n">
-        <v>4.919610204932033</v>
+        <v>8.922482520244779</v>
       </c>
       <c r="F98" t="n">
+        <v>1</v>
+      </c>
+      <c r="G98" t="n">
         <v>600</v>
       </c>
-      <c r="G98" t="n">
+      <c r="H98" t="n">
         <v>0</v>
       </c>
-      <c r="H98" t="n">
-        <v>18.17716503984986</v>
+      <c r="I98" t="n">
+        <v>17.54547096740117</v>
       </c>
     </row>
     <row r="99">
@@ -2937,22 +3233,25 @@
         <v>43843.33333333334</v>
       </c>
       <c r="C99" t="n">
-        <v>26.72305321764393</v>
+        <v>35.04418419323104</v>
       </c>
       <c r="D99" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E99" t="n">
-        <v>8.233516994967829</v>
+        <v>5.095962948514847</v>
       </c>
       <c r="F99" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G99" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H99" t="n">
-        <v>28.96705530231785</v>
+        <v>1</v>
+      </c>
+      <c r="I99" t="n">
+        <v>29.60444968457878</v>
       </c>
     </row>
     <row r="100">
@@ -2963,22 +3262,25 @@
         <v>43843.41666666666</v>
       </c>
       <c r="C100" t="n">
-        <v>38.48923052780626</v>
+        <v>19.1564218335468</v>
       </c>
       <c r="D100" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E100" t="n">
-        <v>2.595280256270758</v>
+        <v>9.665294222641513</v>
       </c>
       <c r="F100" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G100" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H100" t="n">
-        <v>42.69598525439228</v>
+        <v>2</v>
+      </c>
+      <c r="I100" t="n">
+        <v>17.46109704288019</v>
       </c>
     </row>
     <row r="101">
@@ -2989,22 +3291,25 @@
         <v>43843.5</v>
       </c>
       <c r="C101" t="n">
-        <v>15.23082515480901</v>
+        <v>30.20417742038016</v>
       </c>
       <c r="D101" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E101" t="n">
-        <v>6.976254375170901</v>
+        <v>9.251468569105866</v>
       </c>
       <c r="F101" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G101" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H101" t="n">
-        <v>8.052410938933411</v>
+        <v>3</v>
+      </c>
+      <c r="I101" t="n">
+        <v>26.68061191190547</v>
       </c>
     </row>
     <row r="102">
@@ -3015,22 +3320,25 @@
         <v>43843.58333333334</v>
       </c>
       <c r="C102" t="n">
-        <v>37.45118944851756</v>
+        <v>24.6131377083331</v>
       </c>
       <c r="D102" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E102" t="n">
-        <v>8.910848355160873</v>
+        <v>4.42543006110942</v>
       </c>
       <c r="F102" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G102" t="n">
+        <v>120</v>
+      </c>
+      <c r="H102" t="n">
         <v>4</v>
       </c>
-      <c r="H102" t="n">
-        <v>33.47240792830373</v>
+      <c r="I102" t="n">
+        <v>25.18519891500694</v>
       </c>
     </row>
     <row r="103">
@@ -3041,22 +3349,25 @@
         <v>43843.66666666666</v>
       </c>
       <c r="C103" t="n">
-        <v>20.19223591189856</v>
+        <v>32.8571011494496</v>
       </c>
       <c r="D103" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" t="n">
+        <v>8.324612351735736</v>
+      </c>
+      <c r="F103" t="n">
+        <v>2</v>
+      </c>
+      <c r="G103" t="n">
+        <v>120</v>
+      </c>
+      <c r="H103" t="n">
         <v>5</v>
       </c>
-      <c r="E103" t="n">
-        <v>4.869797457849336</v>
-      </c>
-      <c r="F103" t="n">
-        <v>120</v>
-      </c>
-      <c r="G103" t="n">
-        <v>5</v>
-      </c>
-      <c r="H103" t="n">
-        <v>21.18922219211782</v>
+      <c r="I103" t="n">
+        <v>28.95844798076503</v>
       </c>
     </row>
     <row r="104">
@@ -3067,22 +3378,25 @@
         <v>43843.75</v>
       </c>
       <c r="C104" t="n">
-        <v>25.21856614391021</v>
+        <v>27.11039366042559</v>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E104" t="n">
-        <v>5.607875185400009</v>
+        <v>9.827716943160048</v>
       </c>
       <c r="F104" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G104" t="n">
+        <v>120</v>
+      </c>
+      <c r="H104" t="n">
         <v>6</v>
       </c>
-      <c r="H104" t="n">
-        <v>25.04164332016768</v>
+      <c r="I104" t="n">
+        <v>26.9631216350772</v>
       </c>
     </row>
     <row r="105">
@@ -3093,22 +3407,25 @@
         <v>43843.83333333334</v>
       </c>
       <c r="C105" t="n">
-        <v>35.90218118634874</v>
+        <v>26.37074805149618</v>
       </c>
       <c r="D105" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E105" t="n">
-        <v>7.057069833778257</v>
+        <v>4.3483743392893</v>
       </c>
       <c r="F105" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G105" t="n">
+        <v>120</v>
+      </c>
+      <c r="H105" t="n">
         <v>7</v>
       </c>
-      <c r="H105" t="n">
-        <v>38.69317807659363</v>
+      <c r="I105" t="n">
+        <v>28.88446702713882</v>
       </c>
     </row>
     <row r="106">
@@ -3119,22 +3436,25 @@
         <v>43844.25</v>
       </c>
       <c r="C106" t="n">
-        <v>15.57465562475545</v>
+        <v>24.01292950271658</v>
       </c>
       <c r="D106" t="n">
         <v>3</v>
       </c>
       <c r="E106" t="n">
-        <v>5.156465147157393</v>
+        <v>8.634995592518392</v>
       </c>
       <c r="F106" t="n">
+        <v>1</v>
+      </c>
+      <c r="G106" t="n">
         <v>600</v>
       </c>
-      <c r="G106" t="n">
+      <c r="H106" t="n">
         <v>0</v>
       </c>
-      <c r="H106" t="n">
-        <v>14.18543437901888</v>
+      <c r="I106" t="n">
+        <v>28.17758767873188</v>
       </c>
     </row>
     <row r="107">
@@ -3145,22 +3465,25 @@
         <v>43844.33333333334</v>
       </c>
       <c r="C107" t="n">
-        <v>29.95290812679463</v>
+        <v>36.5668397404784</v>
       </c>
       <c r="D107" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E107" t="n">
-        <v>6.004634924866897</v>
+        <v>3.484332752292205</v>
       </c>
       <c r="F107" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G107" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H107" t="n">
-        <v>29.32602552307947</v>
+        <v>1</v>
+      </c>
+      <c r="I107" t="n">
+        <v>35.09342279392959</v>
       </c>
     </row>
     <row r="108">
@@ -3171,22 +3494,25 @@
         <v>43844.41666666666</v>
       </c>
       <c r="C108" t="n">
-        <v>34.95299355245824</v>
+        <v>23.61300629764389</v>
       </c>
       <c r="D108" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E108" t="n">
-        <v>2.283691612407311</v>
+        <v>9.049373424510376</v>
       </c>
       <c r="F108" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G108" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H108" t="n">
-        <v>33.97430545522532</v>
+        <v>2</v>
+      </c>
+      <c r="I108" t="n">
+        <v>22.03992518545854</v>
       </c>
     </row>
     <row r="109">
@@ -3197,22 +3523,25 @@
         <v>43844.5</v>
       </c>
       <c r="C109" t="n">
-        <v>28.76802237141726</v>
+        <v>25.37762649019589</v>
       </c>
       <c r="D109" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E109" t="n">
-        <v>4.493031166501737</v>
+        <v>3.567072014924087</v>
       </c>
       <c r="F109" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G109" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H109" t="n">
-        <v>27.15921036732546</v>
+        <v>3</v>
+      </c>
+      <c r="I109" t="n">
+        <v>35.99060114330825</v>
       </c>
     </row>
     <row r="110">
@@ -3223,22 +3552,25 @@
         <v>43844.58333333334</v>
       </c>
       <c r="C110" t="n">
-        <v>29.0823621077012</v>
+        <v>34.439887159496</v>
       </c>
       <c r="D110" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E110" t="n">
-        <v>9.219571341564649</v>
+        <v>3.80526006196627</v>
       </c>
       <c r="F110" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G110" t="n">
+        <v>120</v>
+      </c>
+      <c r="H110" t="n">
         <v>4</v>
       </c>
-      <c r="H110" t="n">
-        <v>29.59920920340116</v>
+      <c r="I110" t="n">
+        <v>32.49113688287199</v>
       </c>
     </row>
     <row r="111">
@@ -3249,22 +3581,25 @@
         <v>43844.66666666666</v>
       </c>
       <c r="C111" t="n">
-        <v>33.32934180808299</v>
+        <v>24.67414099249808</v>
       </c>
       <c r="D111" t="n">
+        <v>3</v>
+      </c>
+      <c r="E111" t="n">
+        <v>2.415335800405129</v>
+      </c>
+      <c r="F111" t="n">
+        <v>2</v>
+      </c>
+      <c r="G111" t="n">
+        <v>120</v>
+      </c>
+      <c r="H111" t="n">
         <v>5</v>
       </c>
-      <c r="E111" t="n">
-        <v>8.572951218870912</v>
-      </c>
-      <c r="F111" t="n">
-        <v>120</v>
-      </c>
-      <c r="G111" t="n">
-        <v>5</v>
-      </c>
-      <c r="H111" t="n">
-        <v>34.12374208021676</v>
+      <c r="I111" t="n">
+        <v>27.94383194684116</v>
       </c>
     </row>
     <row r="112">
@@ -3275,22 +3610,25 @@
         <v>43844.75</v>
       </c>
       <c r="C112" t="n">
-        <v>37.28593272282355</v>
+        <v>17.35121727234575</v>
       </c>
       <c r="D112" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E112" t="n">
-        <v>3.327844335108963</v>
+        <v>2.392800844745431</v>
       </c>
       <c r="F112" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G112" t="n">
+        <v>120</v>
+      </c>
+      <c r="H112" t="n">
         <v>6</v>
       </c>
-      <c r="H112" t="n">
-        <v>35.79346299615575</v>
+      <c r="I112" t="n">
+        <v>16.99782338615885</v>
       </c>
     </row>
     <row r="113">
@@ -3301,22 +3639,25 @@
         <v>43844.83333333334</v>
       </c>
       <c r="C113" t="n">
-        <v>36.05188288876792</v>
+        <v>16.98895465880684</v>
       </c>
       <c r="D113" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E113" t="n">
-        <v>5.236099690188609</v>
+        <v>4.943137739398478</v>
       </c>
       <c r="F113" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G113" t="n">
+        <v>120</v>
+      </c>
+      <c r="H113" t="n">
         <v>7</v>
       </c>
-      <c r="H113" t="n">
-        <v>30.41081522893631</v>
+      <c r="I113" t="n">
+        <v>22.36954018870551</v>
       </c>
     </row>
     <row r="114">
@@ -3327,22 +3668,25 @@
         <v>43845.25</v>
       </c>
       <c r="C114" t="n">
-        <v>17.72918501414119</v>
+        <v>34.71581865320493</v>
       </c>
       <c r="D114" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E114" t="n">
-        <v>4.247492791039188</v>
+        <v>8.218365029540724</v>
       </c>
       <c r="F114" t="n">
+        <v>1</v>
+      </c>
+      <c r="G114" t="n">
         <v>600</v>
       </c>
-      <c r="G114" t="n">
+      <c r="H114" t="n">
         <v>0</v>
       </c>
-      <c r="H114" t="n">
-        <v>18.59932722963147</v>
+      <c r="I114" t="n">
+        <v>37.51029017398798</v>
       </c>
     </row>
     <row r="115">
@@ -3353,22 +3697,25 @@
         <v>43845.33333333334</v>
       </c>
       <c r="C115" t="n">
-        <v>37.49159539530035</v>
+        <v>26.03190045923757</v>
       </c>
       <c r="D115" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E115" t="n">
-        <v>7.406799711995165</v>
+        <v>7.68273792093438</v>
       </c>
       <c r="F115" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G115" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H115" t="n">
-        <v>36.73332248660277</v>
+        <v>1</v>
+      </c>
+      <c r="I115" t="n">
+        <v>24.46125679369164</v>
       </c>
     </row>
     <row r="116">
@@ -3379,22 +3726,25 @@
         <v>43845.41666666666</v>
       </c>
       <c r="C116" t="n">
-        <v>29.15258267470136</v>
+        <v>30.34722017819718</v>
       </c>
       <c r="D116" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E116" t="n">
-        <v>9.3876763051277</v>
+        <v>6.91636618409854</v>
       </c>
       <c r="F116" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="G116" t="n">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="H116" t="n">
-        <v>26.52473205136334</v>
+        <v>2</v>
+      </c>
+      <c r="I116" t="n">
+        <v>33.40524542946081</v>
       </c>
     </row>
     <row r="117">
@@ -3405,22 +3755,25 @@
         <v>43845.5</v>
       </c>
       <c r="C117" t="n">
-        <v>16.93875796797695</v>
+        <v>38.66510238981864</v>
       </c>
       <c r="D117" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E117" t="n">
-        <v>2.368109957140023</v>
+        <v>2.569369986995622</v>
       </c>
       <c r="F117" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G117" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H117" t="n">
-        <v>13.7316750692246</v>
+        <v>3</v>
+      </c>
+      <c r="I117" t="n">
+        <v>42.41552645938534</v>
       </c>
     </row>
     <row r="118">
@@ -3431,22 +3784,25 @@
         <v>43845.58333333334</v>
       </c>
       <c r="C118" t="n">
-        <v>32.23388663494847</v>
+        <v>18.16162068059963</v>
       </c>
       <c r="D118" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E118" t="n">
-        <v>8.343078346024829</v>
+        <v>2.389079162615802</v>
       </c>
       <c r="F118" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G118" t="n">
+        <v>120</v>
+      </c>
+      <c r="H118" t="n">
         <v>4</v>
       </c>
-      <c r="H118" t="n">
-        <v>36.30652366108536</v>
+      <c r="I118" t="n">
+        <v>11.88625764031978</v>
       </c>
     </row>
     <row r="119">
@@ -3457,22 +3813,25 @@
         <v>43845.66666666666</v>
       </c>
       <c r="C119" t="n">
-        <v>21.24236910031977</v>
+        <v>30.12749553576078</v>
       </c>
       <c r="D119" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E119" t="n">
-        <v>6.82301657207702</v>
+        <v>7.098700405604906</v>
       </c>
       <c r="F119" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G119" t="n">
+        <v>120</v>
+      </c>
+      <c r="H119" t="n">
         <v>5</v>
       </c>
-      <c r="H119" t="n">
-        <v>17.29861252393087</v>
+      <c r="I119" t="n">
+        <v>34.72756221754631</v>
       </c>
     </row>
     <row r="120">
@@ -3483,22 +3842,25 @@
         <v>43845.75</v>
       </c>
       <c r="C120" t="n">
-        <v>15.18424251439844</v>
+        <v>17.03919004859481</v>
       </c>
       <c r="D120" t="n">
+        <v>12</v>
+      </c>
+      <c r="E120" t="n">
+        <v>9.994174337557238</v>
+      </c>
+      <c r="F120" t="n">
+        <v>3</v>
+      </c>
+      <c r="G120" t="n">
+        <v>120</v>
+      </c>
+      <c r="H120" t="n">
         <v>6</v>
       </c>
-      <c r="E120" t="n">
-        <v>7.703103368395971</v>
-      </c>
-      <c r="F120" t="n">
-        <v>120</v>
-      </c>
-      <c r="G120" t="n">
-        <v>6</v>
-      </c>
-      <c r="H120" t="n">
-        <v>17.45705641876806</v>
+      <c r="I120" t="n">
+        <v>16.87216142106744</v>
       </c>
     </row>
     <row r="121">
@@ -3509,22 +3871,25 @@
         <v>43845.83333333334</v>
       </c>
       <c r="C121" t="n">
-        <v>23.10206776129281</v>
+        <v>30.94090589965226</v>
       </c>
       <c r="D121" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E121" t="n">
-        <v>2.134689491929308</v>
+        <v>4.246351130496029</v>
       </c>
       <c r="F121" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="G121" t="n">
+        <v>120</v>
+      </c>
+      <c r="H121" t="n">
         <v>7</v>
       </c>
-      <c r="H121" t="n">
-        <v>21.03669298867911</v>
+      <c r="I121" t="n">
+        <v>31.59787741569124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fake data and regression attempt, 0.86 accuracy
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -420,13 +420,13 @@
         <v>43831.25</v>
       </c>
       <c r="C2" t="n">
-        <v>24.29313615024982</v>
+        <v>24.68458296627677</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
-        <v>12.92870947433298</v>
+        <v>10.72105897926874</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -438,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>28.73826072901844</v>
+        <v>43.30598580980615</v>
       </c>
     </row>
     <row r="3">
@@ -449,13 +449,13 @@
         <v>43831.33333333334</v>
       </c>
       <c r="C3" t="n">
-        <v>31.24499645577075</v>
+        <v>20.02023871535856</v>
       </c>
       <c r="D3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="n">
-        <v>7.568998926582053</v>
+        <v>9.85947266139987</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -467,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>28.5496780174663</v>
+        <v>45.30775472115359</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         <v>43831.41666666666</v>
       </c>
       <c r="C4" t="n">
-        <v>16.57588561510314</v>
+        <v>39.24977452539517</v>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="n">
-        <v>9.632486666674508</v>
+        <v>4.512211968035874</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -496,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>15.89456882962867</v>
+        <v>54.19665589993484</v>
       </c>
     </row>
     <row r="5">
@@ -507,13 +507,13 @@
         <v>43831.5</v>
       </c>
       <c r="C5" t="n">
-        <v>39.79025244514101</v>
+        <v>27.50271697234307</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>10.63054535911128</v>
+        <v>11.26820545322557</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -525,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>42.65422640502907</v>
+        <v>37.62361860250174</v>
       </c>
     </row>
     <row r="6">
@@ -536,13 +536,13 @@
         <v>43831.58333333334</v>
       </c>
       <c r="C6" t="n">
-        <v>20.89069516493274</v>
+        <v>35.04959148943401</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>8.986496381014168</v>
+        <v>8.370734539177283</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
@@ -554,7 +554,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="n">
-        <v>26.30374623519725</v>
+        <v>47.03510735618401</v>
       </c>
     </row>
     <row r="7">
@@ -565,13 +565,13 @@
         <v>43831.66666666666</v>
       </c>
       <c r="C7" t="n">
-        <v>36.76180295788764</v>
+        <v>39.25666901396127</v>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" t="n">
-        <v>5.472511757457013</v>
+        <v>11.55770461451318</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -583,7 +583,7 @@
         <v>5</v>
       </c>
       <c r="I7" t="n">
-        <v>34.6283601187202</v>
+        <v>55.4513533243301</v>
       </c>
     </row>
     <row r="8">
@@ -594,13 +594,13 @@
         <v>43831.75</v>
       </c>
       <c r="C8" t="n">
-        <v>16.91108062134489</v>
+        <v>17.16282160551393</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>8.158875058447252</v>
+        <v>6.981840833407463</v>
       </c>
       <c r="F8" t="n">
         <v>3</v>
@@ -612,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="I8" t="n">
-        <v>18.19624848087675</v>
+        <v>20.19880851893287</v>
       </c>
     </row>
     <row r="9">
@@ -623,13 +623,13 @@
         <v>43831.83333333334</v>
       </c>
       <c r="C9" t="n">
-        <v>36.47881791100824</v>
+        <v>16.71078265812217</v>
       </c>
       <c r="D9" t="n">
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>9.637877307308839</v>
+        <v>11.34204262720077</v>
       </c>
       <c r="F9" t="n">
         <v>3</v>
@@ -641,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="I9" t="n">
-        <v>35.82320590361794</v>
+        <v>26.87155064134883</v>
       </c>
     </row>
     <row r="10">
@@ -652,13 +652,13 @@
         <v>43832.25</v>
       </c>
       <c r="C10" t="n">
-        <v>37.06423310678308</v>
+        <v>19.59801231252413</v>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>16.86887127642347</v>
+        <v>9.765386658330765</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>34.57831393433858</v>
+        <v>39.77548206804324</v>
       </c>
     </row>
     <row r="11">
@@ -681,13 +681,13 @@
         <v>43832.33333333334</v>
       </c>
       <c r="C11" t="n">
-        <v>28.51621108111954</v>
+        <v>15.64049060073585</v>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E11" t="n">
-        <v>10.31725337419957</v>
+        <v>15.29978806404818</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -699,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>33.859506715206</v>
+        <v>39.73155293139424</v>
       </c>
     </row>
     <row r="12">
@@ -710,13 +710,13 @@
         <v>43832.41666666666</v>
       </c>
       <c r="C12" t="n">
-        <v>35.82088116762284</v>
+        <v>23.69516045293241</v>
       </c>
       <c r="D12" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" t="n">
-        <v>10.40841331768636</v>
+        <v>9.067932088535432</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
@@ -728,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="I12" t="n">
-        <v>39.78992786349485</v>
+        <v>42.558487836196</v>
       </c>
     </row>
     <row r="13">
@@ -739,13 +739,13 @@
         <v>43832.5</v>
       </c>
       <c r="C13" t="n">
-        <v>18.64921742967775</v>
+        <v>39.59053203028413</v>
       </c>
       <c r="D13" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E13" t="n">
-        <v>10.37372715525254</v>
+        <v>13.46084912139769</v>
       </c>
       <c r="F13" t="n">
         <v>2</v>
@@ -757,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="I13" t="n">
-        <v>17.73447078305759</v>
+        <v>54.11222036696818</v>
       </c>
     </row>
     <row r="14">
@@ -768,13 +768,13 @@
         <v>43832.58333333334</v>
       </c>
       <c r="C14" t="n">
-        <v>39.26086835048179</v>
+        <v>37.90526372711832</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>6.792736710451226</v>
+        <v>13.10045288806427</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
@@ -786,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="I14" t="n">
-        <v>39.71022378025742</v>
+        <v>48.47484390388642</v>
       </c>
     </row>
     <row r="15">
@@ -797,13 +797,13 @@
         <v>43832.66666666666</v>
       </c>
       <c r="C15" t="n">
-        <v>28.00493598784782</v>
+        <v>38.7528340490731</v>
       </c>
       <c r="D15" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>7.507004504937508</v>
+        <v>7.662794062173793</v>
       </c>
       <c r="F15" t="n">
         <v>2</v>
@@ -815,7 +815,7 @@
         <v>5</v>
       </c>
       <c r="I15" t="n">
-        <v>28.75009467692834</v>
+        <v>51.48830898384289</v>
       </c>
     </row>
     <row r="16">
@@ -826,13 +826,13 @@
         <v>43832.75</v>
       </c>
       <c r="C16" t="n">
-        <v>27.84344961118814</v>
+        <v>22.34342354739917</v>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" t="n">
-        <v>6.282784858813833</v>
+        <v>9.094209585010258</v>
       </c>
       <c r="F16" t="n">
         <v>3</v>
@@ -844,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="I16" t="n">
-        <v>23.73082303373685</v>
+        <v>22.69401388406132</v>
       </c>
     </row>
     <row r="17">
@@ -855,13 +855,13 @@
         <v>43832.83333333334</v>
       </c>
       <c r="C17" t="n">
-        <v>32.33437364569709</v>
+        <v>24.15275808771658</v>
       </c>
       <c r="D17" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E17" t="n">
-        <v>8.964401904650854</v>
+        <v>8.820317769295952</v>
       </c>
       <c r="F17" t="n">
         <v>3</v>
@@ -873,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="I17" t="n">
-        <v>23.91652957168504</v>
+        <v>32.57158990156472</v>
       </c>
     </row>
     <row r="18">
@@ -884,13 +884,13 @@
         <v>43833.25</v>
       </c>
       <c r="C18" t="n">
-        <v>26.26381882856622</v>
+        <v>18.47285982414637</v>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>6.31074689809917</v>
+        <v>13.15188815631362</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>23.92493929918091</v>
+        <v>31.17762890433076</v>
       </c>
     </row>
     <row r="19">
@@ -913,13 +913,13 @@
         <v>43833.33333333334</v>
       </c>
       <c r="C19" t="n">
-        <v>33.10636813297205</v>
+        <v>29.73542989463269</v>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E19" t="n">
-        <v>12.79940646606746</v>
+        <v>13.37506680669195</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>33.47119172251085</v>
+        <v>43.65032122719644</v>
       </c>
     </row>
     <row r="20">
@@ -942,13 +942,13 @@
         <v>43833.41666666666</v>
       </c>
       <c r="C20" t="n">
-        <v>22.33555357461322</v>
+        <v>33.32383889953611</v>
       </c>
       <c r="D20" t="n">
         <v>5</v>
       </c>
       <c r="E20" t="n">
-        <v>8.849108442587188</v>
+        <v>8.731727605623497</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
@@ -960,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>27.00227178731703</v>
+        <v>49.28974653556594</v>
       </c>
     </row>
     <row r="21">
@@ -971,13 +971,13 @@
         <v>43833.5</v>
       </c>
       <c r="C21" t="n">
-        <v>25.33149756214747</v>
+        <v>32.60254372784095</v>
       </c>
       <c r="D21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" t="n">
-        <v>4.490079261328061</v>
+        <v>13.8017710413948</v>
       </c>
       <c r="F21" t="n">
         <v>2</v>
@@ -989,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="I21" t="n">
-        <v>30.47846671716892</v>
+        <v>39.06215525169763</v>
       </c>
     </row>
     <row r="22">
@@ -1000,13 +1000,13 @@
         <v>43833.58333333334</v>
       </c>
       <c r="C22" t="n">
-        <v>18.30856897050323</v>
+        <v>23.9470847823107</v>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E22" t="n">
-        <v>9.772378327047642</v>
+        <v>14.66124519170342</v>
       </c>
       <c r="F22" t="n">
         <v>2</v>
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="I22" t="n">
-        <v>13.75254076142235</v>
+        <v>37.3539584372061</v>
       </c>
     </row>
     <row r="23">
@@ -1029,13 +1029,13 @@
         <v>43833.66666666666</v>
       </c>
       <c r="C23" t="n">
-        <v>16.74302587720289</v>
+        <v>37.70451233283868</v>
       </c>
       <c r="D23" t="n">
         <v>4</v>
       </c>
       <c r="E23" t="n">
-        <v>9.208138775296279</v>
+        <v>5.974730622384832</v>
       </c>
       <c r="F23" t="n">
         <v>2</v>
@@ -1047,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="I23" t="n">
-        <v>9.141979541074868</v>
+        <v>46.63033009743575</v>
       </c>
     </row>
     <row r="24">
@@ -1058,13 +1058,13 @@
         <v>43833.75</v>
       </c>
       <c r="C24" t="n">
-        <v>39.99633520778998</v>
+        <v>24.7292498911487</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E24" t="n">
-        <v>9.346516675771596</v>
+        <v>12.55909723723446</v>
       </c>
       <c r="F24" t="n">
         <v>3</v>
@@ -1076,7 +1076,7 @@
         <v>6</v>
       </c>
       <c r="I24" t="n">
-        <v>35.62959438086908</v>
+        <v>29.16385449953796</v>
       </c>
     </row>
     <row r="25">
@@ -1087,13 +1087,13 @@
         <v>43833.83333333334</v>
       </c>
       <c r="C25" t="n">
-        <v>34.43199433638819</v>
+        <v>32.37562812730332</v>
       </c>
       <c r="D25" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6.866058746496197</v>
+        <v>11.77841637291388</v>
       </c>
       <c r="F25" t="n">
         <v>3</v>
@@ -1105,7 +1105,7 @@
         <v>7</v>
       </c>
       <c r="I25" t="n">
-        <v>41.97610204994006</v>
+        <v>37.66738832370478</v>
       </c>
     </row>
     <row r="26">
@@ -1116,13 +1116,13 @@
         <v>43834.25</v>
       </c>
       <c r="C26" t="n">
-        <v>25.8501803541987</v>
+        <v>32.04563865847324</v>
       </c>
       <c r="D26" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E26" t="n">
-        <v>14.19196871851656</v>
+        <v>11.02872029465495</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
@@ -1134,7 +1134,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>30.2619455612119</v>
+        <v>50.34532907442751</v>
       </c>
     </row>
     <row r="27">
@@ -1145,13 +1145,13 @@
         <v>43834.33333333334</v>
       </c>
       <c r="C27" t="n">
-        <v>39.00108957790926</v>
+        <v>19.1215153810435</v>
       </c>
       <c r="D27" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E27" t="n">
-        <v>13.3923965854979</v>
+        <v>11.62106926602791</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="I27" t="n">
-        <v>38.12505624474527</v>
+        <v>38.15764258727523</v>
       </c>
     </row>
     <row r="28">
@@ -1174,13 +1174,13 @@
         <v>43834.41666666666</v>
       </c>
       <c r="C28" t="n">
-        <v>29.36613687224721</v>
+        <v>17.86528199164494</v>
       </c>
       <c r="D28" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E28" t="n">
-        <v>4.919458419209095</v>
+        <v>8.278741406211834</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
@@ -1192,7 +1192,7 @@
         <v>2</v>
       </c>
       <c r="I28" t="n">
-        <v>27.41404868847076</v>
+        <v>38.12364101900564</v>
       </c>
     </row>
     <row r="29">
@@ -1203,13 +1203,13 @@
         <v>43834.5</v>
       </c>
       <c r="C29" t="n">
-        <v>19.84823966676918</v>
+        <v>39.14172268677248</v>
       </c>
       <c r="D29" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E29" t="n">
-        <v>11.1723383545437</v>
+        <v>9.599690858069476</v>
       </c>
       <c r="F29" t="n">
         <v>2</v>
@@ -1221,7 +1221,7 @@
         <v>3</v>
       </c>
       <c r="I29" t="n">
-        <v>20.2001598325857</v>
+        <v>53.49895825468166</v>
       </c>
     </row>
     <row r="30">
@@ -1232,13 +1232,13 @@
         <v>43834.58333333334</v>
       </c>
       <c r="C30" t="n">
-        <v>36.17106520442152</v>
+        <v>35.56595608967881</v>
       </c>
       <c r="D30" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E30" t="n">
-        <v>12.52228442215416</v>
+        <v>11.34336096864551</v>
       </c>
       <c r="F30" t="n">
         <v>2</v>
@@ -1250,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="I30" t="n">
-        <v>37.26631735387833</v>
+        <v>48.27773568895563</v>
       </c>
     </row>
     <row r="31">
@@ -1261,13 +1261,13 @@
         <v>43834.66666666666</v>
       </c>
       <c r="C31" t="n">
-        <v>33.388800058274</v>
+        <v>35.00250993923301</v>
       </c>
       <c r="D31" t="n">
         <v>4</v>
       </c>
       <c r="E31" t="n">
-        <v>8.011488432276382</v>
+        <v>8.261057761134092</v>
       </c>
       <c r="F31" t="n">
         <v>2</v>
@@ -1279,7 +1279,7 @@
         <v>5</v>
       </c>
       <c r="I31" t="n">
-        <v>31.82763982690491</v>
+        <v>50.04752636032443</v>
       </c>
     </row>
     <row r="32">
@@ -1290,13 +1290,13 @@
         <v>43834.75</v>
       </c>
       <c r="C32" t="n">
-        <v>30.48004543554835</v>
+        <v>30.68877610839311</v>
       </c>
       <c r="D32" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E32" t="n">
-        <v>11.24999204241738</v>
+        <v>10.76205612526483</v>
       </c>
       <c r="F32" t="n">
         <v>3</v>
@@ -1308,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="I32" t="n">
-        <v>28.46540513668388</v>
+        <v>36.21505360865656</v>
       </c>
     </row>
     <row r="33">
@@ -1319,13 +1319,13 @@
         <v>43834.83333333334</v>
       </c>
       <c r="C33" t="n">
-        <v>21.14756848178063</v>
+        <v>31.55790170453247</v>
       </c>
       <c r="D33" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>10.28503647309506</v>
+        <v>9.4871295355778</v>
       </c>
       <c r="F33" t="n">
         <v>3</v>
@@ -1337,7 +1337,7 @@
         <v>7</v>
       </c>
       <c r="I33" t="n">
-        <v>18.12510431026293</v>
+        <v>35.22892193487101</v>
       </c>
     </row>
     <row r="34">
@@ -1348,13 +1348,13 @@
         <v>43835.25</v>
       </c>
       <c r="C34" t="n">
-        <v>37.75072105059502</v>
+        <v>32.38962256420714</v>
       </c>
       <c r="D34" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>14.35607732607096</v>
+        <v>4.397471137960934</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
@@ -1366,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>42.43295517396242</v>
+        <v>61.07655448633314</v>
       </c>
     </row>
     <row r="35">
@@ -1377,13 +1377,13 @@
         <v>43835.33333333334</v>
       </c>
       <c r="C35" t="n">
-        <v>27.6264908400888</v>
+        <v>17.81338176746825</v>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E35" t="n">
-        <v>12.93156551598796</v>
+        <v>10.55644444798965</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
@@ -1395,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>32.23958316434635</v>
+        <v>43.16031178839951</v>
       </c>
     </row>
     <row r="36">
@@ -1406,13 +1406,13 @@
         <v>43835.41666666666</v>
       </c>
       <c r="C36" t="n">
-        <v>21.61222742624165</v>
+        <v>30.27318140779622</v>
       </c>
       <c r="D36" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E36" t="n">
-        <v>10.21041882577405</v>
+        <v>9.823925255485252</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
@@ -1424,7 +1424,7 @@
         <v>2</v>
       </c>
       <c r="I36" t="n">
-        <v>23.68697056454544</v>
+        <v>47.57291550277976</v>
       </c>
     </row>
     <row r="37">
@@ -1435,13 +1435,13 @@
         <v>43835.5</v>
       </c>
       <c r="C37" t="n">
-        <v>18.5558182309482</v>
+        <v>17.40258220482682</v>
       </c>
       <c r="D37" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E37" t="n">
-        <v>9.55484896114916</v>
+        <v>8.039312411790382</v>
       </c>
       <c r="F37" t="n">
         <v>2</v>
@@ -1453,7 +1453,7 @@
         <v>3</v>
       </c>
       <c r="I37" t="n">
-        <v>22.26568072103498</v>
+        <v>21.78947791800704</v>
       </c>
     </row>
     <row r="38">
@@ -1464,13 +1464,13 @@
         <v>43835.58333333334</v>
       </c>
       <c r="C38" t="n">
-        <v>23.44518900407621</v>
+        <v>20.66458997461516</v>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E38" t="n">
-        <v>8.004127263779342</v>
+        <v>7.393909594124132</v>
       </c>
       <c r="F38" t="n">
         <v>2</v>
@@ -1482,7 +1482,7 @@
         <v>4</v>
       </c>
       <c r="I38" t="n">
-        <v>23.63262610615944</v>
+        <v>32.12907303730949</v>
       </c>
     </row>
     <row r="39">
@@ -1493,13 +1493,13 @@
         <v>43835.66666666666</v>
       </c>
       <c r="C39" t="n">
-        <v>18.88377412533169</v>
+        <v>32.81458946110438</v>
       </c>
       <c r="D39" t="n">
         <v>4</v>
       </c>
       <c r="E39" t="n">
-        <v>9.981239000481413</v>
+        <v>9.463257461566268</v>
       </c>
       <c r="F39" t="n">
         <v>2</v>
@@ -1511,7 +1511,7 @@
         <v>5</v>
       </c>
       <c r="I39" t="n">
-        <v>19.43089049817567</v>
+        <v>36.29239274552222</v>
       </c>
     </row>
     <row r="40">
@@ -1522,13 +1522,13 @@
         <v>43835.75</v>
       </c>
       <c r="C40" t="n">
-        <v>32.29329202400442</v>
+        <v>35.64819764647089</v>
       </c>
       <c r="D40" t="n">
         <v>6</v>
       </c>
       <c r="E40" t="n">
-        <v>5.479274351646241</v>
+        <v>9.247533404034053</v>
       </c>
       <c r="F40" t="n">
         <v>3</v>
@@ -1540,7 +1540,7 @@
         <v>6</v>
       </c>
       <c r="I40" t="n">
-        <v>32.88561035665517</v>
+        <v>41.36602251753007</v>
       </c>
     </row>
     <row r="41">
@@ -1551,13 +1551,13 @@
         <v>43835.83333333334</v>
       </c>
       <c r="C41" t="n">
-        <v>35.93234102584633</v>
+        <v>30.99565554624044</v>
       </c>
       <c r="D41" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E41" t="n">
-        <v>11.19472280456478</v>
+        <v>13.67454730434242</v>
       </c>
       <c r="F41" t="n">
         <v>3</v>
@@ -1569,7 +1569,7 @@
         <v>7</v>
       </c>
       <c r="I41" t="n">
-        <v>30.22309845411579</v>
+        <v>44.55227172002527</v>
       </c>
     </row>
     <row r="42">
@@ -1580,13 +1580,13 @@
         <v>43836.25</v>
       </c>
       <c r="C42" t="n">
-        <v>33.54166743923672</v>
+        <v>28.91853278396279</v>
       </c>
       <c r="D42" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E42" t="n">
-        <v>16.53641324204862</v>
+        <v>8.56199830863399</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -1598,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>36.06493137837701</v>
+        <v>46.03149587198703</v>
       </c>
     </row>
     <row r="43">
@@ -1609,13 +1609,13 @@
         <v>43836.33333333334</v>
       </c>
       <c r="C43" t="n">
-        <v>20.98918683347267</v>
+        <v>34.14216140491732</v>
       </c>
       <c r="D43" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E43" t="n">
-        <v>7.775656004905221</v>
+        <v>6.188812299968577</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="I43" t="n">
-        <v>20.52428306821027</v>
+        <v>54.01252783799014</v>
       </c>
     </row>
     <row r="44">
@@ -1638,13 +1638,13 @@
         <v>43836.41666666666</v>
       </c>
       <c r="C44" t="n">
-        <v>29.51711748219459</v>
+        <v>39.60942227384746</v>
       </c>
       <c r="D44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E44" t="n">
-        <v>9.541355258877857</v>
+        <v>12.23244938831991</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -1656,7 +1656,7 @@
         <v>2</v>
       </c>
       <c r="I44" t="n">
-        <v>24.86501206287637</v>
+        <v>53.59277135002485</v>
       </c>
     </row>
     <row r="45">
@@ -1667,13 +1667,13 @@
         <v>43836.5</v>
       </c>
       <c r="C45" t="n">
-        <v>21.37193496331484</v>
+        <v>18.70995951521692</v>
       </c>
       <c r="D45" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>10.50694946965162</v>
+        <v>10.70030356363322</v>
       </c>
       <c r="F45" t="n">
         <v>2</v>
@@ -1685,7 +1685,7 @@
         <v>3</v>
       </c>
       <c r="I45" t="n">
-        <v>13.58427518068532</v>
+        <v>19.31864682112037</v>
       </c>
     </row>
     <row r="46">
@@ -1696,13 +1696,13 @@
         <v>43836.58333333334</v>
       </c>
       <c r="C46" t="n">
-        <v>35.48989473799177</v>
+        <v>28.94328380322344</v>
       </c>
       <c r="D46" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E46" t="n">
-        <v>10.22220377096667</v>
+        <v>8.653442821425148</v>
       </c>
       <c r="F46" t="n">
         <v>2</v>
@@ -1714,7 +1714,7 @@
         <v>4</v>
       </c>
       <c r="I46" t="n">
-        <v>29.76870952818151</v>
+        <v>42.78108430851555</v>
       </c>
     </row>
     <row r="47">
@@ -1725,13 +1725,13 @@
         <v>43836.66666666666</v>
       </c>
       <c r="C47" t="n">
-        <v>19.01700396622452</v>
+        <v>17.12817066544321</v>
       </c>
       <c r="D47" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E47" t="n">
-        <v>8.52032062169204</v>
+        <v>8.277007609091594</v>
       </c>
       <c r="F47" t="n">
         <v>2</v>
@@ -1743,7 +1743,7 @@
         <v>5</v>
       </c>
       <c r="I47" t="n">
-        <v>29.04859246949426</v>
+        <v>23.02279744748066</v>
       </c>
     </row>
     <row r="48">
@@ -1754,13 +1754,13 @@
         <v>43836.75</v>
       </c>
       <c r="C48" t="n">
-        <v>39.51307729586324</v>
+        <v>34.76167112275835</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>9.698496718030238</v>
+        <v>8.671265367951239</v>
       </c>
       <c r="F48" t="n">
         <v>3</v>
@@ -1772,7 +1772,7 @@
         <v>6</v>
       </c>
       <c r="I48" t="n">
-        <v>37.00455622069911</v>
+        <v>42.72659826494364</v>
       </c>
     </row>
     <row r="49">
@@ -1783,13 +1783,13 @@
         <v>43836.83333333334</v>
       </c>
       <c r="C49" t="n">
-        <v>17.5440115498284</v>
+        <v>32.36662846465072</v>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E49" t="n">
-        <v>14.47697896321272</v>
+        <v>6.294255404874923</v>
       </c>
       <c r="F49" t="n">
         <v>3</v>
@@ -1801,7 +1801,7 @@
         <v>7</v>
       </c>
       <c r="I49" t="n">
-        <v>16.67537303042361</v>
+        <v>36.55257248544581</v>
       </c>
     </row>
     <row r="50">
@@ -1812,13 +1812,13 @@
         <v>43837.25</v>
       </c>
       <c r="C50" t="n">
-        <v>18.41086922947417</v>
+        <v>23.35018142663671</v>
       </c>
       <c r="D50" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E50" t="n">
-        <v>4.320861967486161</v>
+        <v>10.22454121387226</v>
       </c>
       <c r="F50" t="n">
         <v>1</v>
@@ -1830,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="n">
-        <v>19.39628869521412</v>
+        <v>48.6243116688587</v>
       </c>
     </row>
     <row r="51">
@@ -1841,13 +1841,13 @@
         <v>43837.33333333334</v>
       </c>
       <c r="C51" t="n">
-        <v>35.85605247015252</v>
+        <v>36.87910093818326</v>
       </c>
       <c r="D51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E51" t="n">
-        <v>13.64231889688116</v>
+        <v>14.2599133239793</v>
       </c>
       <c r="F51" t="n">
         <v>1</v>
@@ -1859,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="I51" t="n">
-        <v>41.52422799391207</v>
+        <v>41.0416194227866</v>
       </c>
     </row>
     <row r="52">
@@ -1870,13 +1870,13 @@
         <v>43837.41666666666</v>
       </c>
       <c r="C52" t="n">
-        <v>32.83556945821789</v>
+        <v>32.48414650656269</v>
       </c>
       <c r="D52" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E52" t="n">
-        <v>9.549432071144778</v>
+        <v>14.36564115664542</v>
       </c>
       <c r="F52" t="n">
         <v>1</v>
@@ -1888,7 +1888,7 @@
         <v>2</v>
       </c>
       <c r="I52" t="n">
-        <v>34.1148948937647</v>
+        <v>39.68399496457682</v>
       </c>
     </row>
     <row r="53">
@@ -1899,13 +1899,13 @@
         <v>43837.5</v>
       </c>
       <c r="C53" t="n">
-        <v>20.22393475971348</v>
+        <v>22.35009553165384</v>
       </c>
       <c r="D53" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E53" t="n">
-        <v>12.30458421954664</v>
+        <v>13.33345071279841</v>
       </c>
       <c r="F53" t="n">
         <v>2</v>
@@ -1917,7 +1917,7 @@
         <v>3</v>
       </c>
       <c r="I53" t="n">
-        <v>21.6143725223985</v>
+        <v>24.26605675353739</v>
       </c>
     </row>
     <row r="54">
@@ -1928,13 +1928,13 @@
         <v>43837.58333333334</v>
       </c>
       <c r="C54" t="n">
-        <v>15.14116255481383</v>
+        <v>17.20278230614784</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>12.20992866333012</v>
+        <v>9.132378039153906</v>
       </c>
       <c r="F54" t="n">
         <v>2</v>
@@ -1946,7 +1946,7 @@
         <v>4</v>
       </c>
       <c r="I54" t="n">
-        <v>8.504718325780148</v>
+        <v>31.34940413446614</v>
       </c>
     </row>
     <row r="55">
@@ -1957,13 +1957,13 @@
         <v>43837.66666666666</v>
       </c>
       <c r="C55" t="n">
-        <v>35.97101309787987</v>
+        <v>33.01989560476231</v>
       </c>
       <c r="D55" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>13.06682447101636</v>
+        <v>6.136942263535488</v>
       </c>
       <c r="F55" t="n">
         <v>2</v>
@@ -1975,7 +1975,7 @@
         <v>5</v>
       </c>
       <c r="I55" t="n">
-        <v>38.74591873746875</v>
+        <v>34.79820576109447</v>
       </c>
     </row>
     <row r="56">
@@ -1986,13 +1986,13 @@
         <v>43837.75</v>
       </c>
       <c r="C56" t="n">
-        <v>28.38572043167265</v>
+        <v>29.41033929415547</v>
       </c>
       <c r="D56" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>9.587824507919141</v>
+        <v>5.841544350144225</v>
       </c>
       <c r="F56" t="n">
         <v>3</v>
@@ -2004,7 +2004,7 @@
         <v>6</v>
       </c>
       <c r="I56" t="n">
-        <v>25.8570066511171</v>
+        <v>38.28422598847472</v>
       </c>
     </row>
     <row r="57">
@@ -2015,13 +2015,13 @@
         <v>43837.83333333334</v>
       </c>
       <c r="C57" t="n">
-        <v>27.1113335217782</v>
+        <v>27.0175080434407</v>
       </c>
       <c r="D57" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E57" t="n">
-        <v>10.85029485418642</v>
+        <v>10.16341019380062</v>
       </c>
       <c r="F57" t="n">
         <v>3</v>
@@ -2033,7 +2033,7 @@
         <v>7</v>
       </c>
       <c r="I57" t="n">
-        <v>25.55815989320431</v>
+        <v>28.06845438358401</v>
       </c>
     </row>
     <row r="58">
@@ -2044,13 +2044,13 @@
         <v>43838.25</v>
       </c>
       <c r="C58" t="n">
-        <v>20.74752545896658</v>
+        <v>26.31476254430673</v>
       </c>
       <c r="D58" t="n">
         <v>12</v>
       </c>
       <c r="E58" t="n">
-        <v>8.316506511859846</v>
+        <v>10.19017055436121</v>
       </c>
       <c r="F58" t="n">
         <v>1</v>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>28.32840539441782</v>
+        <v>49.66007326601405</v>
       </c>
     </row>
     <row r="59">
@@ -2073,13 +2073,13 @@
         <v>43838.33333333334</v>
       </c>
       <c r="C59" t="n">
-        <v>37.56609680218598</v>
+        <v>27.96106167859546</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E59" t="n">
-        <v>12.47328948087564</v>
+        <v>13.16904920258681</v>
       </c>
       <c r="F59" t="n">
         <v>1</v>
@@ -2091,7 +2091,7 @@
         <v>1</v>
       </c>
       <c r="I59" t="n">
-        <v>36.02783796575749</v>
+        <v>43.60763629849331</v>
       </c>
     </row>
     <row r="60">
@@ -2102,13 +2102,13 @@
         <v>43838.41666666666</v>
       </c>
       <c r="C60" t="n">
-        <v>38.9615973533311</v>
+        <v>28.2184649786814</v>
       </c>
       <c r="D60" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E60" t="n">
-        <v>8.543361934470576</v>
+        <v>11.94478294796737</v>
       </c>
       <c r="F60" t="n">
         <v>1</v>
@@ -2120,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="I60" t="n">
-        <v>36.96870888723658</v>
+        <v>47.79352053627697</v>
       </c>
     </row>
     <row r="61">
@@ -2131,13 +2131,13 @@
         <v>43838.5</v>
       </c>
       <c r="C61" t="n">
-        <v>32.22903983624074</v>
+        <v>34.48788777177316</v>
       </c>
       <c r="D61" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E61" t="n">
-        <v>8.509841704388888</v>
+        <v>5.101378371587581</v>
       </c>
       <c r="F61" t="n">
         <v>2</v>
@@ -2149,7 +2149,7 @@
         <v>3</v>
       </c>
       <c r="I61" t="n">
-        <v>28.85317624037307</v>
+        <v>52.97831119128166</v>
       </c>
     </row>
     <row r="62">
@@ -2160,13 +2160,13 @@
         <v>43838.58333333334</v>
       </c>
       <c r="C62" t="n">
-        <v>22.5222666280569</v>
+        <v>37.21439361863837</v>
       </c>
       <c r="D62" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E62" t="n">
-        <v>10.54972149558778</v>
+        <v>8.167832112058232</v>
       </c>
       <c r="F62" t="n">
         <v>2</v>
@@ -2178,7 +2178,7 @@
         <v>4</v>
       </c>
       <c r="I62" t="n">
-        <v>16.60180106119505</v>
+        <v>53.30180647775627</v>
       </c>
     </row>
     <row r="63">
@@ -2189,13 +2189,13 @@
         <v>43838.66666666666</v>
       </c>
       <c r="C63" t="n">
-        <v>39.42084890547811</v>
+        <v>18.79721900125215</v>
       </c>
       <c r="D63" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E63" t="n">
-        <v>8.630974465058365</v>
+        <v>12.38686873793227</v>
       </c>
       <c r="F63" t="n">
         <v>2</v>
@@ -2207,7 +2207,7 @@
         <v>5</v>
       </c>
       <c r="I63" t="n">
-        <v>47.65314169134651</v>
+        <v>26.99096179826045</v>
       </c>
     </row>
     <row r="64">
@@ -2218,13 +2218,13 @@
         <v>43838.75</v>
       </c>
       <c r="C64" t="n">
-        <v>35.0485880193595</v>
+        <v>30.05822301673632</v>
       </c>
       <c r="D64" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E64" t="n">
-        <v>10.74810405500934</v>
+        <v>14.1021961943423</v>
       </c>
       <c r="F64" t="n">
         <v>3</v>
@@ -2236,7 +2236,7 @@
         <v>6</v>
       </c>
       <c r="I64" t="n">
-        <v>36.58755108119902</v>
+        <v>35.06137833957938</v>
       </c>
     </row>
     <row r="65">
@@ -2247,13 +2247,13 @@
         <v>43838.83333333334</v>
       </c>
       <c r="C65" t="n">
-        <v>32.48477415936748</v>
+        <v>37.02401108785894</v>
       </c>
       <c r="D65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E65" t="n">
-        <v>12.7317349247735</v>
+        <v>14.75801580993844</v>
       </c>
       <c r="F65" t="n">
         <v>3</v>
@@ -2265,7 +2265,7 @@
         <v>7</v>
       </c>
       <c r="I65" t="n">
-        <v>38.74865390544053</v>
+        <v>43.96850427542255</v>
       </c>
     </row>
     <row r="66">
@@ -2276,13 +2276,13 @@
         <v>43839.25</v>
       </c>
       <c r="C66" t="n">
-        <v>24.05526287290711</v>
+        <v>39.58218023850412</v>
       </c>
       <c r="D66" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E66" t="n">
-        <v>9.562817868407821</v>
+        <v>11.6351261003108</v>
       </c>
       <c r="F66" t="n">
         <v>1</v>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="I66" t="n">
-        <v>22.73397849468312</v>
+        <v>55.27554722973302</v>
       </c>
     </row>
     <row r="67">
@@ -2305,13 +2305,13 @@
         <v>43839.33333333334</v>
       </c>
       <c r="C67" t="n">
-        <v>21.98784515994465</v>
+        <v>15.78929182800446</v>
       </c>
       <c r="D67" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E67" t="n">
-        <v>17.42188978919394</v>
+        <v>14.38048108119962</v>
       </c>
       <c r="F67" t="n">
         <v>1</v>
@@ -2323,7 +2323,7 @@
         <v>1</v>
       </c>
       <c r="I67" t="n">
-        <v>27.30738744116726</v>
+        <v>39.63082470733205</v>
       </c>
     </row>
     <row r="68">
@@ -2334,13 +2334,13 @@
         <v>43839.41666666666</v>
       </c>
       <c r="C68" t="n">
-        <v>33.42765132079047</v>
+        <v>19.4004072726814</v>
       </c>
       <c r="D68" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E68" t="n">
-        <v>11.2493401863451</v>
+        <v>11.23166396922674</v>
       </c>
       <c r="F68" t="n">
         <v>1</v>
@@ -2352,7 +2352,7 @@
         <v>2</v>
       </c>
       <c r="I68" t="n">
-        <v>35.22700825918321</v>
+        <v>44.94289440616463</v>
       </c>
     </row>
     <row r="69">
@@ -2363,13 +2363,13 @@
         <v>43839.5</v>
       </c>
       <c r="C69" t="n">
-        <v>36.49956831900086</v>
+        <v>26.30781456922124</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E69" t="n">
-        <v>12.27577088575747</v>
+        <v>7.703271451620713</v>
       </c>
       <c r="F69" t="n">
         <v>2</v>
@@ -2381,7 +2381,7 @@
         <v>3</v>
       </c>
       <c r="I69" t="n">
-        <v>39.51931356910812</v>
+        <v>45.67134297783176</v>
       </c>
     </row>
     <row r="70">
@@ -2392,13 +2392,13 @@
         <v>43839.58333333334</v>
       </c>
       <c r="C70" t="n">
-        <v>38.42171815260254</v>
+        <v>39.15430752337094</v>
       </c>
       <c r="D70" t="n">
         <v>9</v>
       </c>
       <c r="E70" t="n">
-        <v>14.72649143016391</v>
+        <v>12.13488559927579</v>
       </c>
       <c r="F70" t="n">
         <v>2</v>
@@ -2410,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="I70" t="n">
-        <v>33.38340524973962</v>
+        <v>52.0772328438463</v>
       </c>
     </row>
     <row r="71">
@@ -2421,13 +2421,13 @@
         <v>43839.66666666666</v>
       </c>
       <c r="C71" t="n">
-        <v>36.86127087924375</v>
+        <v>27.09510762635853</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
       </c>
       <c r="E71" t="n">
-        <v>6.676190505602188</v>
+        <v>8.123469811246929</v>
       </c>
       <c r="F71" t="n">
         <v>2</v>
@@ -2439,7 +2439,7 @@
         <v>5</v>
       </c>
       <c r="I71" t="n">
-        <v>42.31333853956222</v>
+        <v>37.40749203138962</v>
       </c>
     </row>
     <row r="72">
@@ -2450,13 +2450,13 @@
         <v>43839.75</v>
       </c>
       <c r="C72" t="n">
-        <v>32.92046128528839</v>
+        <v>38.91748490459034</v>
       </c>
       <c r="D72" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E72" t="n">
-        <v>8.347008807375884</v>
+        <v>9.775321818061153</v>
       </c>
       <c r="F72" t="n">
         <v>3</v>
@@ -2468,7 +2468,7 @@
         <v>6</v>
       </c>
       <c r="I72" t="n">
-        <v>35.84230347326695</v>
+        <v>44.1550128516356</v>
       </c>
     </row>
     <row r="73">
@@ -2479,13 +2479,13 @@
         <v>43839.83333333334</v>
       </c>
       <c r="C73" t="n">
-        <v>15.81242818616261</v>
+        <v>38.08605402517259</v>
       </c>
       <c r="D73" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E73" t="n">
-        <v>9.223005783371406</v>
+        <v>1.662134294538596</v>
       </c>
       <c r="F73" t="n">
         <v>3</v>
@@ -2497,7 +2497,7 @@
         <v>7</v>
       </c>
       <c r="I73" t="n">
-        <v>17.086848214469</v>
+        <v>50.22668671135414</v>
       </c>
     </row>
     <row r="74">
@@ -2508,13 +2508,13 @@
         <v>43840.25</v>
       </c>
       <c r="C74" t="n">
-        <v>22.97791126828</v>
+        <v>22.47629761257127</v>
       </c>
       <c r="D74" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10.09637116259935</v>
+        <v>7.210228030925128</v>
       </c>
       <c r="F74" t="n">
         <v>1</v>
@@ -2526,7 +2526,7 @@
         <v>0</v>
       </c>
       <c r="I74" t="n">
-        <v>22.46960668374212</v>
+        <v>40.4074764412153</v>
       </c>
     </row>
     <row r="75">
@@ -2537,13 +2537,13 @@
         <v>43840.33333333334</v>
       </c>
       <c r="C75" t="n">
-        <v>37.86465876934741</v>
+        <v>38.28566537877117</v>
       </c>
       <c r="D75" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10.05684801378138</v>
+        <v>11.19702965507893</v>
       </c>
       <c r="F75" t="n">
         <v>1</v>
@@ -2555,7 +2555,7 @@
         <v>1</v>
       </c>
       <c r="I75" t="n">
-        <v>45.25017758716657</v>
+        <v>64.44545177272261</v>
       </c>
     </row>
     <row r="76">
@@ -2566,13 +2566,13 @@
         <v>43840.41666666666</v>
       </c>
       <c r="C76" t="n">
-        <v>26.96956950776877</v>
+        <v>37.87548735967673</v>
       </c>
       <c r="D76" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E76" t="n">
-        <v>8.536699891506411</v>
+        <v>12.10979100047746</v>
       </c>
       <c r="F76" t="n">
         <v>1</v>
@@ -2584,7 +2584,7 @@
         <v>2</v>
       </c>
       <c r="I76" t="n">
-        <v>27.98208948137151</v>
+        <v>60.53622772106845</v>
       </c>
     </row>
     <row r="77">
@@ -2595,13 +2595,13 @@
         <v>43840.5</v>
       </c>
       <c r="C77" t="n">
-        <v>25.4238271353333</v>
+        <v>15.69166233729827</v>
       </c>
       <c r="D77" t="n">
         <v>12</v>
       </c>
       <c r="E77" t="n">
-        <v>8.418885348295367</v>
+        <v>6.627893740344196</v>
       </c>
       <c r="F77" t="n">
         <v>2</v>
@@ -2613,7 +2613,7 @@
         <v>3</v>
       </c>
       <c r="I77" t="n">
-        <v>28.68379126870512</v>
+        <v>31.29334468128831</v>
       </c>
     </row>
     <row r="78">
@@ -2624,13 +2624,13 @@
         <v>43840.58333333334</v>
       </c>
       <c r="C78" t="n">
-        <v>26.24006611082001</v>
+        <v>37.4355485097863</v>
       </c>
       <c r="D78" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E78" t="n">
-        <v>13.49170105203206</v>
+        <v>11.98520229498089</v>
       </c>
       <c r="F78" t="n">
         <v>2</v>
@@ -2642,7 +2642,7 @@
         <v>4</v>
       </c>
       <c r="I78" t="n">
-        <v>18.53861779878077</v>
+        <v>43.02263063059032</v>
       </c>
     </row>
     <row r="79">
@@ -2653,13 +2653,13 @@
         <v>43840.66666666666</v>
       </c>
       <c r="C79" t="n">
-        <v>16.36946118739285</v>
+        <v>26.77907599017513</v>
       </c>
       <c r="D79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E79" t="n">
-        <v>18.46416194623107</v>
+        <v>11.90641099780318</v>
       </c>
       <c r="F79" t="n">
         <v>2</v>
@@ -2671,7 +2671,7 @@
         <v>5</v>
       </c>
       <c r="I79" t="n">
-        <v>7.689713301905234</v>
+        <v>36.32521932797847</v>
       </c>
     </row>
     <row r="80">
@@ -2682,13 +2682,13 @@
         <v>43840.75</v>
       </c>
       <c r="C80" t="n">
-        <v>21.88220213815389</v>
+        <v>25.78367733536169</v>
       </c>
       <c r="D80" t="n">
         <v>11</v>
       </c>
       <c r="E80" t="n">
-        <v>7.278809457924555</v>
+        <v>8.314358037316159</v>
       </c>
       <c r="F80" t="n">
         <v>3</v>
@@ -2700,7 +2700,7 @@
         <v>6</v>
       </c>
       <c r="I80" t="n">
-        <v>18.77249513833209</v>
+        <v>37.44732072191903</v>
       </c>
     </row>
     <row r="81">
@@ -2711,13 +2711,13 @@
         <v>43840.83333333334</v>
       </c>
       <c r="C81" t="n">
-        <v>26.95777834251896</v>
+        <v>26.96828774424591</v>
       </c>
       <c r="D81" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E81" t="n">
-        <v>11.44580713906454</v>
+        <v>13.70745939174912</v>
       </c>
       <c r="F81" t="n">
         <v>3</v>
@@ -2729,7 +2729,7 @@
         <v>7</v>
       </c>
       <c r="I81" t="n">
-        <v>28.33836106545932</v>
+        <v>32.80653354518837</v>
       </c>
     </row>
     <row r="82">
@@ -2740,13 +2740,13 @@
         <v>43841.25</v>
       </c>
       <c r="C82" t="n">
-        <v>19.64632560166987</v>
+        <v>26.50771580904895</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E82" t="n">
-        <v>10.91284065120992</v>
+        <v>18.20148390554819</v>
       </c>
       <c r="F82" t="n">
         <v>1</v>
@@ -2758,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="I82" t="n">
-        <v>19.15787454551159</v>
+        <v>45.23078343070996</v>
       </c>
     </row>
     <row r="83">
@@ -2769,13 +2769,13 @@
         <v>43841.33333333334</v>
       </c>
       <c r="C83" t="n">
-        <v>27.33436077048697</v>
+        <v>25.27402821688447</v>
       </c>
       <c r="D83" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E83" t="n">
-        <v>14.4055886606981</v>
+        <v>6.836204050852075</v>
       </c>
       <c r="F83" t="n">
         <v>1</v>
@@ -2787,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="I83" t="n">
-        <v>26.42736459867906</v>
+        <v>50.81611882160189</v>
       </c>
     </row>
     <row r="84">
@@ -2798,13 +2798,13 @@
         <v>43841.41666666666</v>
       </c>
       <c r="C84" t="n">
-        <v>31.26788024943864</v>
+        <v>22.20781072775534</v>
       </c>
       <c r="D84" t="n">
         <v>8</v>
       </c>
       <c r="E84" t="n">
-        <v>10.04671766797391</v>
+        <v>9.29153149722144</v>
       </c>
       <c r="F84" t="n">
         <v>1</v>
@@ -2816,7 +2816,7 @@
         <v>2</v>
       </c>
       <c r="I84" t="n">
-        <v>33.11277112650018</v>
+        <v>42.69529459255966</v>
       </c>
     </row>
     <row r="85">
@@ -2827,13 +2827,13 @@
         <v>43841.5</v>
       </c>
       <c r="C85" t="n">
-        <v>28.65044965423899</v>
+        <v>27.6629628697766</v>
       </c>
       <c r="D85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E85" t="n">
-        <v>10.98530911320486</v>
+        <v>12.30044956309004</v>
       </c>
       <c r="F85" t="n">
         <v>2</v>
@@ -2845,7 +2845,7 @@
         <v>3</v>
       </c>
       <c r="I85" t="n">
-        <v>27.78030426038073</v>
+        <v>45.01756069458451</v>
       </c>
     </row>
     <row r="86">
@@ -2856,13 +2856,13 @@
         <v>43841.58333333334</v>
       </c>
       <c r="C86" t="n">
-        <v>23.10634604459005</v>
+        <v>35.83479529006989</v>
       </c>
       <c r="D86" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8.126193370215425</v>
+        <v>10.29727595538661</v>
       </c>
       <c r="F86" t="n">
         <v>2</v>
@@ -2874,7 +2874,7 @@
         <v>4</v>
       </c>
       <c r="I86" t="n">
-        <v>25.70641334691618</v>
+        <v>54.37241314774705</v>
       </c>
     </row>
     <row r="87">
@@ -2885,13 +2885,13 @@
         <v>43841.66666666666</v>
       </c>
       <c r="C87" t="n">
-        <v>25.7280122438596</v>
+        <v>25.93234231502837</v>
       </c>
       <c r="D87" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E87" t="n">
-        <v>11.35240252868968</v>
+        <v>15.9712613110443</v>
       </c>
       <c r="F87" t="n">
         <v>2</v>
@@ -2903,7 +2903,7 @@
         <v>5</v>
       </c>
       <c r="I87" t="n">
-        <v>22.75133227169932</v>
+        <v>34.74844380511422</v>
       </c>
     </row>
     <row r="88">
@@ -2914,13 +2914,13 @@
         <v>43841.75</v>
       </c>
       <c r="C88" t="n">
-        <v>38.67752894198804</v>
+        <v>20.73567843169316</v>
       </c>
       <c r="D88" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E88" t="n">
-        <v>10.79521408911829</v>
+        <v>6.271000962385155</v>
       </c>
       <c r="F88" t="n">
         <v>3</v>
@@ -2932,7 +2932,7 @@
         <v>6</v>
       </c>
       <c r="I88" t="n">
-        <v>37.65245383813249</v>
+        <v>20.69517175448632</v>
       </c>
     </row>
     <row r="89">
@@ -2943,13 +2943,13 @@
         <v>43841.83333333334</v>
       </c>
       <c r="C89" t="n">
-        <v>37.19358397958001</v>
+        <v>38.52428219997261</v>
       </c>
       <c r="D89" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E89" t="n">
-        <v>4.952933589917446</v>
+        <v>12.81014872881964</v>
       </c>
       <c r="F89" t="n">
         <v>3</v>
@@ -2961,7 +2961,7 @@
         <v>7</v>
       </c>
       <c r="I89" t="n">
-        <v>37.64775578282471</v>
+        <v>50.86224184873492</v>
       </c>
     </row>
     <row r="90">
@@ -2972,13 +2972,13 @@
         <v>43842.25</v>
       </c>
       <c r="C90" t="n">
-        <v>39.87288218082546</v>
+        <v>39.70512921300518</v>
       </c>
       <c r="D90" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>12.03679471697322</v>
+        <v>12.12589092564929</v>
       </c>
       <c r="F90" t="n">
         <v>1</v>
@@ -2990,7 +2990,7 @@
         <v>0</v>
       </c>
       <c r="I90" t="n">
-        <v>37.31735341554089</v>
+        <v>56.2544705444445</v>
       </c>
     </row>
     <row r="91">
@@ -3001,13 +3001,13 @@
         <v>43842.33333333334</v>
       </c>
       <c r="C91" t="n">
-        <v>32.32339401679653</v>
+        <v>27.23383434265716</v>
       </c>
       <c r="D91" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E91" t="n">
-        <v>9.357528011633539</v>
+        <v>11.22843009668144</v>
       </c>
       <c r="F91" t="n">
         <v>1</v>
@@ -3019,7 +3019,7 @@
         <v>1</v>
       </c>
       <c r="I91" t="n">
-        <v>30.76185852161878</v>
+        <v>50.70061484144786</v>
       </c>
     </row>
     <row r="92">
@@ -3030,13 +3030,13 @@
         <v>43842.41666666666</v>
       </c>
       <c r="C92" t="n">
-        <v>22.81670960343533</v>
+        <v>24.26404003439929</v>
       </c>
       <c r="D92" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E92" t="n">
-        <v>9.747146588593989</v>
+        <v>8.453892129367969</v>
       </c>
       <c r="F92" t="n">
         <v>1</v>
@@ -3048,7 +3048,7 @@
         <v>2</v>
       </c>
       <c r="I92" t="n">
-        <v>23.68386638743541</v>
+        <v>33.30618399658587</v>
       </c>
     </row>
     <row r="93">
@@ -3059,13 +3059,13 @@
         <v>43842.5</v>
       </c>
       <c r="C93" t="n">
-        <v>38.79377406759733</v>
+        <v>22.05641354106434</v>
       </c>
       <c r="D93" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E93" t="n">
-        <v>8.59033345760419</v>
+        <v>10.58570371567064</v>
       </c>
       <c r="F93" t="n">
         <v>2</v>
@@ -3077,7 +3077,7 @@
         <v>3</v>
       </c>
       <c r="I93" t="n">
-        <v>33.79236735188237</v>
+        <v>32.77573333459454</v>
       </c>
     </row>
     <row r="94">
@@ -3088,13 +3088,13 @@
         <v>43842.58333333334</v>
       </c>
       <c r="C94" t="n">
-        <v>22.46014265080488</v>
+        <v>33.04837244214421</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E94" t="n">
-        <v>5.501651771224608</v>
+        <v>6.155361166682358</v>
       </c>
       <c r="F94" t="n">
         <v>2</v>
@@ -3106,7 +3106,7 @@
         <v>4</v>
       </c>
       <c r="I94" t="n">
-        <v>17.1301425232417</v>
+        <v>49.11947883379852</v>
       </c>
     </row>
     <row r="95">
@@ -3117,13 +3117,13 @@
         <v>43842.66666666666</v>
       </c>
       <c r="C95" t="n">
-        <v>21.66687944035245</v>
+        <v>37.61773250273068</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6.943929699059597</v>
+        <v>8.963555318303712</v>
       </c>
       <c r="F95" t="n">
         <v>2</v>
@@ -3135,7 +3135,7 @@
         <v>5</v>
       </c>
       <c r="I95" t="n">
-        <v>17.32604459748017</v>
+        <v>52.40351952197178</v>
       </c>
     </row>
     <row r="96">
@@ -3146,13 +3146,13 @@
         <v>43842.75</v>
       </c>
       <c r="C96" t="n">
-        <v>34.00167937869107</v>
+        <v>29.40585451286736</v>
       </c>
       <c r="D96" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10.22628180934065</v>
+        <v>11.16449507170002</v>
       </c>
       <c r="F96" t="n">
         <v>3</v>
@@ -3164,7 +3164,7 @@
         <v>6</v>
       </c>
       <c r="I96" t="n">
-        <v>29.63114678500331</v>
+        <v>38.59764389039712</v>
       </c>
     </row>
     <row r="97">
@@ -3175,13 +3175,13 @@
         <v>43842.83333333334</v>
       </c>
       <c r="C97" t="n">
-        <v>35.35722028862072</v>
+        <v>39.60331003624884</v>
       </c>
       <c r="D97" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E97" t="n">
-        <v>8.204200302733277</v>
+        <v>11.74249413109769</v>
       </c>
       <c r="F97" t="n">
         <v>3</v>
@@ -3193,7 +3193,7 @@
         <v>7</v>
       </c>
       <c r="I97" t="n">
-        <v>38.81964664163884</v>
+        <v>46.45341870647057</v>
       </c>
     </row>
     <row r="98">
@@ -3204,13 +3204,13 @@
         <v>43843.25</v>
       </c>
       <c r="C98" t="n">
-        <v>38.95368187766165</v>
+        <v>29.73290380617076</v>
       </c>
       <c r="D98" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E98" t="n">
-        <v>7.025483134698701</v>
+        <v>6.106454159049745</v>
       </c>
       <c r="F98" t="n">
         <v>1</v>
@@ -3222,7 +3222,7 @@
         <v>0</v>
       </c>
       <c r="I98" t="n">
-        <v>40.7871034925056</v>
+        <v>44.4220499249444</v>
       </c>
     </row>
     <row r="99">
@@ -3233,13 +3233,13 @@
         <v>43843.33333333334</v>
       </c>
       <c r="C99" t="n">
-        <v>37.73334734035947</v>
+        <v>17.1490037367756</v>
       </c>
       <c r="D99" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E99" t="n">
-        <v>14.41351337693193</v>
+        <v>10.19645662111145</v>
       </c>
       <c r="F99" t="n">
         <v>1</v>
@@ -3251,7 +3251,7 @@
         <v>1</v>
       </c>
       <c r="I99" t="n">
-        <v>42.88261333635987</v>
+        <v>26.90234790729273</v>
       </c>
     </row>
     <row r="100">
@@ -3262,13 +3262,13 @@
         <v>43843.41666666666</v>
       </c>
       <c r="C100" t="n">
-        <v>15.06438179642979</v>
+        <v>31.98834178138284</v>
       </c>
       <c r="D100" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E100" t="n">
-        <v>5.508735667810853</v>
+        <v>7.41641013968862</v>
       </c>
       <c r="F100" t="n">
         <v>1</v>
@@ -3280,7 +3280,7 @@
         <v>2</v>
       </c>
       <c r="I100" t="n">
-        <v>7.774782282179153</v>
+        <v>47.99133846593993</v>
       </c>
     </row>
     <row r="101">
@@ -3291,13 +3291,13 @@
         <v>43843.5</v>
       </c>
       <c r="C101" t="n">
-        <v>35.60696160387734</v>
+        <v>22.54960208435103</v>
       </c>
       <c r="D101" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E101" t="n">
-        <v>13.53282162663232</v>
+        <v>8.81948239810394</v>
       </c>
       <c r="F101" t="n">
         <v>2</v>
@@ -3309,7 +3309,7 @@
         <v>3</v>
       </c>
       <c r="I101" t="n">
-        <v>34.92005062391125</v>
+        <v>36.47278026558035</v>
       </c>
     </row>
     <row r="102">
@@ -3320,13 +3320,13 @@
         <v>43843.58333333334</v>
       </c>
       <c r="C102" t="n">
-        <v>18.56364365680889</v>
+        <v>23.66123568734898</v>
       </c>
       <c r="D102" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E102" t="n">
-        <v>6.028889721894269</v>
+        <v>13.08951301175225</v>
       </c>
       <c r="F102" t="n">
         <v>2</v>
@@ -3338,7 +3338,7 @@
         <v>4</v>
       </c>
       <c r="I102" t="n">
-        <v>18.6118821511128</v>
+        <v>37.50259199212521</v>
       </c>
     </row>
     <row r="103">
@@ -3349,13 +3349,13 @@
         <v>43843.66666666666</v>
       </c>
       <c r="C103" t="n">
-        <v>30.55556133652398</v>
+        <v>35.19154845400929</v>
       </c>
       <c r="D103" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E103" t="n">
-        <v>9.232709365540934</v>
+        <v>10.11988559075239</v>
       </c>
       <c r="F103" t="n">
         <v>2</v>
@@ -3367,7 +3367,7 @@
         <v>5</v>
       </c>
       <c r="I103" t="n">
-        <v>27.7142400868056</v>
+        <v>45.50727796310763</v>
       </c>
     </row>
     <row r="104">
@@ -3378,13 +3378,13 @@
         <v>43843.75</v>
       </c>
       <c r="C104" t="n">
-        <v>18.60553026309968</v>
+        <v>35.01273076782333</v>
       </c>
       <c r="D104" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E104" t="n">
-        <v>10.88924341978868</v>
+        <v>12.66649136673226</v>
       </c>
       <c r="F104" t="n">
         <v>3</v>
@@ -3396,7 +3396,7 @@
         <v>6</v>
       </c>
       <c r="I104" t="n">
-        <v>21.81272279716646</v>
+        <v>43.91132750366494</v>
       </c>
     </row>
     <row r="105">
@@ -3407,13 +3407,13 @@
         <v>43843.83333333334</v>
       </c>
       <c r="C105" t="n">
-        <v>19.59184434992997</v>
+        <v>35.64100285380761</v>
       </c>
       <c r="D105" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E105" t="n">
-        <v>16.0251142430167</v>
+        <v>8.608027152415104</v>
       </c>
       <c r="F105" t="n">
         <v>3</v>
@@ -3425,7 +3425,7 @@
         <v>7</v>
       </c>
       <c r="I105" t="n">
-        <v>16.97215363497336</v>
+        <v>41.41551720739515</v>
       </c>
     </row>
     <row r="106">
@@ -3436,13 +3436,13 @@
         <v>43844.25</v>
       </c>
       <c r="C106" t="n">
-        <v>21.62196054834271</v>
+        <v>31.82538706187379</v>
       </c>
       <c r="D106" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E106" t="n">
-        <v>6.027601432072646</v>
+        <v>8.147948832976896</v>
       </c>
       <c r="F106" t="n">
         <v>1</v>
@@ -3454,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="I106" t="n">
-        <v>18.35295431766057</v>
+        <v>46.32296180727639</v>
       </c>
     </row>
     <row r="107">
@@ -3465,13 +3465,13 @@
         <v>43844.33333333334</v>
       </c>
       <c r="C107" t="n">
-        <v>15.58200271187137</v>
+        <v>15.16909706311383</v>
       </c>
       <c r="D107" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E107" t="n">
-        <v>7.313275616437686</v>
+        <v>11.31244766373987</v>
       </c>
       <c r="F107" t="n">
         <v>1</v>
@@ -3483,7 +3483,7 @@
         <v>1</v>
       </c>
       <c r="I107" t="n">
-        <v>14.54498721467092</v>
+        <v>32.24196463219871</v>
       </c>
     </row>
     <row r="108">
@@ -3494,13 +3494,13 @@
         <v>43844.41666666666</v>
       </c>
       <c r="C108" t="n">
-        <v>18.8638296861868</v>
+        <v>24.59252807759063</v>
       </c>
       <c r="D108" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E108" t="n">
-        <v>8.525084762847946</v>
+        <v>9.657763738618536</v>
       </c>
       <c r="F108" t="n">
         <v>1</v>
@@ -3512,7 +3512,7 @@
         <v>2</v>
       </c>
       <c r="I108" t="n">
-        <v>26.35310834656251</v>
+        <v>48.68017712849488</v>
       </c>
     </row>
     <row r="109">
@@ -3523,13 +3523,13 @@
         <v>43844.5</v>
       </c>
       <c r="C109" t="n">
-        <v>37.29660476755065</v>
+        <v>22.85627157461182</v>
       </c>
       <c r="D109" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E109" t="n">
-        <v>0.9789537161303201</v>
+        <v>4.374358520011684</v>
       </c>
       <c r="F109" t="n">
         <v>2</v>
@@ -3541,7 +3541,7 @@
         <v>3</v>
       </c>
       <c r="I109" t="n">
-        <v>32.98627623146695</v>
+        <v>36.79572901092141</v>
       </c>
     </row>
     <row r="110">
@@ -3552,13 +3552,13 @@
         <v>43844.58333333334</v>
       </c>
       <c r="C110" t="n">
-        <v>15.16327169825504</v>
+        <v>30.9693899734784</v>
       </c>
       <c r="D110" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E110" t="n">
-        <v>13.2938498644035</v>
+        <v>8.753191002876665</v>
       </c>
       <c r="F110" t="n">
         <v>2</v>
@@ -3570,7 +3570,7 @@
         <v>4</v>
       </c>
       <c r="I110" t="n">
-        <v>26.65035163264342</v>
+        <v>49.15762301178495</v>
       </c>
     </row>
     <row r="111">
@@ -3581,13 +3581,13 @@
         <v>43844.66666666666</v>
       </c>
       <c r="C111" t="n">
-        <v>20.43664813899914</v>
+        <v>28.40274165647171</v>
       </c>
       <c r="D111" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E111" t="n">
-        <v>14.39348259849866</v>
+        <v>4.608372309415858</v>
       </c>
       <c r="F111" t="n">
         <v>2</v>
@@ -3599,7 +3599,7 @@
         <v>5</v>
       </c>
       <c r="I111" t="n">
-        <v>17.07411985111754</v>
+        <v>37.06134047553509</v>
       </c>
     </row>
     <row r="112">
@@ -3610,13 +3610,13 @@
         <v>43844.75</v>
       </c>
       <c r="C112" t="n">
-        <v>31.34904504590516</v>
+        <v>28.52188190063687</v>
       </c>
       <c r="D112" t="n">
         <v>2</v>
       </c>
       <c r="E112" t="n">
-        <v>5.391600132843688</v>
+        <v>9.242157620153238</v>
       </c>
       <c r="F112" t="n">
         <v>3</v>
@@ -3628,7 +3628,7 @@
         <v>6</v>
       </c>
       <c r="I112" t="n">
-        <v>34.88277405254112</v>
+        <v>30.2808025344473</v>
       </c>
     </row>
     <row r="113">
@@ -3639,13 +3639,13 @@
         <v>43844.83333333334</v>
       </c>
       <c r="C113" t="n">
-        <v>15.41844578075593</v>
+        <v>35.33315127059941</v>
       </c>
       <c r="D113" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E113" t="n">
-        <v>6.377063271893924</v>
+        <v>13.76211833849931</v>
       </c>
       <c r="F113" t="n">
         <v>3</v>
@@ -3657,7 +3657,7 @@
         <v>7</v>
       </c>
       <c r="I113" t="n">
-        <v>20.48692530186254</v>
+        <v>39.213298493595</v>
       </c>
     </row>
     <row r="114">
@@ -3668,13 +3668,13 @@
         <v>43845.25</v>
       </c>
       <c r="C114" t="n">
-        <v>17.82039970433195</v>
+        <v>23.58933736981319</v>
       </c>
       <c r="D114" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E114" t="n">
-        <v>7.006898746593312</v>
+        <v>11.10707428122939</v>
       </c>
       <c r="F114" t="n">
         <v>1</v>
@@ -3686,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="I114" t="n">
-        <v>12.42456116851092</v>
+        <v>39.31052845119628</v>
       </c>
     </row>
     <row r="115">
@@ -3697,13 +3697,13 @@
         <v>43845.33333333334</v>
       </c>
       <c r="C115" t="n">
-        <v>34.68304679687614</v>
+        <v>22.05121581254452</v>
       </c>
       <c r="D115" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E115" t="n">
-        <v>14.20830169796747</v>
+        <v>2.599459444131162</v>
       </c>
       <c r="F115" t="n">
         <v>1</v>
@@ -3715,7 +3715,7 @@
         <v>1</v>
       </c>
       <c r="I115" t="n">
-        <v>37.6836485372223</v>
+        <v>42.20062127132707</v>
       </c>
     </row>
     <row r="116">
@@ -3726,13 +3726,13 @@
         <v>43845.41666666666</v>
       </c>
       <c r="C116" t="n">
-        <v>29.9888725117883</v>
+        <v>18.15488472261904</v>
       </c>
       <c r="D116" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E116" t="n">
-        <v>7.139881488162464</v>
+        <v>1.539744945002811</v>
       </c>
       <c r="F116" t="n">
         <v>1</v>
@@ -3744,7 +3744,7 @@
         <v>2</v>
       </c>
       <c r="I116" t="n">
-        <v>26.92954971274434</v>
+        <v>42.07942649003241</v>
       </c>
     </row>
     <row r="117">
@@ -3755,13 +3755,13 @@
         <v>43845.5</v>
       </c>
       <c r="C117" t="n">
-        <v>33.17934201632721</v>
+        <v>17.22568628598596</v>
       </c>
       <c r="D117" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E117" t="n">
-        <v>13.28226854466335</v>
+        <v>6.264246283046194</v>
       </c>
       <c r="F117" t="n">
         <v>2</v>
@@ -3773,7 +3773,7 @@
         <v>3</v>
       </c>
       <c r="I117" t="n">
-        <v>32.58044760342257</v>
+        <v>22.97692852135047</v>
       </c>
     </row>
     <row r="118">
@@ -3784,13 +3784,13 @@
         <v>43845.58333333334</v>
       </c>
       <c r="C118" t="n">
-        <v>27.60982521079514</v>
+        <v>25.10935525835491</v>
       </c>
       <c r="D118" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E118" t="n">
-        <v>10.68157541121439</v>
+        <v>7.469965373429396</v>
       </c>
       <c r="F118" t="n">
         <v>2</v>
@@ -3802,7 +3802,7 @@
         <v>4</v>
       </c>
       <c r="I118" t="n">
-        <v>34.03800881774572</v>
+        <v>34.64227462439293</v>
       </c>
     </row>
     <row r="119">
@@ -3813,13 +3813,13 @@
         <v>43845.66666666666</v>
       </c>
       <c r="C119" t="n">
-        <v>35.63476559161714</v>
+        <v>38.76523047157384</v>
       </c>
       <c r="D119" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E119" t="n">
-        <v>13.8950794003453</v>
+        <v>12.03116541102904</v>
       </c>
       <c r="F119" t="n">
         <v>2</v>
@@ -3831,7 +3831,7 @@
         <v>5</v>
       </c>
       <c r="I119" t="n">
-        <v>27.57200972899902</v>
+        <v>55.06004329601165</v>
       </c>
     </row>
     <row r="120">
@@ -3842,13 +3842,13 @@
         <v>43845.75</v>
       </c>
       <c r="C120" t="n">
-        <v>21.49795355355855</v>
+        <v>35.39808058161677</v>
       </c>
       <c r="D120" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E120" t="n">
-        <v>13.38665634133164</v>
+        <v>2.305677205044249</v>
       </c>
       <c r="F120" t="n">
         <v>3</v>
@@ -3860,7 +3860,7 @@
         <v>6</v>
       </c>
       <c r="I120" t="n">
-        <v>21.31990857258061</v>
+        <v>37.03167807296117</v>
       </c>
     </row>
     <row r="121">
@@ -3871,13 +3871,13 @@
         <v>43845.83333333334</v>
       </c>
       <c r="C121" t="n">
-        <v>17.69217615053828</v>
+        <v>16.19882392480669</v>
       </c>
       <c r="D121" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E121" t="n">
-        <v>10.94763161223627</v>
+        <v>10.9590917041832</v>
       </c>
       <c r="F121" t="n">
         <v>3</v>
@@ -3889,7 +3889,7 @@
         <v>7</v>
       </c>
       <c r="I121" t="n">
-        <v>14.12822141198187</v>
+        <v>25.65121835108208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>